<commit_message>
Update automatico via Actualizar 05-17-2020 22-15-38
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{41ADEA5A-6120-48CF-8775-8582F2C175E3}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F83CAD7E-D42F-4826-8299-7A10BD477BF9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="Q17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V23" sqref="V23"/>
+      <pane ySplit="1" topLeftCell="T12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2020 16-21-10
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="T12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W22" sqref="W22"/>
+      <pane ySplit="1" topLeftCell="O2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2020 19-21-29
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F83CAD7E-D42F-4826-8299-7A10BD477BF9}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46D35F55-0837-4980-95C8-1F5934711C2F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="O2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <pane ySplit="1" topLeftCell="S34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -1789,10 +1789,10 @@
         <v>36</v>
       </c>
       <c r="V2" s="2">
-        <v>14.5923</v>
+        <v>15.5989</v>
       </c>
       <c r="W2" s="2">
-        <v>-88.5822</v>
+        <v>-87.208799999999997</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -1857,10 +1857,10 @@
         <v>37</v>
       </c>
       <c r="V3" s="2">
-        <v>14.5924</v>
+        <v>15.7836</v>
       </c>
       <c r="W3" s="2">
-        <v>-88.582700000000003</v>
+        <v>-86.792500000000004</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -1925,10 +1925,10 @@
         <v>38</v>
       </c>
       <c r="V4" s="2">
-        <v>14.594900000000001</v>
+        <v>15.784800000000001</v>
       </c>
       <c r="W4" s="2">
-        <v>-88.581699999999998</v>
+        <v>-86.792900000000003</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -1993,10 +1993,10 @@
         <v>39</v>
       </c>
       <c r="V5" s="2">
-        <v>14.5952</v>
+        <v>15.7849</v>
       </c>
       <c r="W5" s="2">
-        <v>-88.581599999999995</v>
+        <v>-86.791899999999998</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -2061,10 +2061,10 @@
         <v>45</v>
       </c>
       <c r="V6" s="2">
-        <v>14.547599999999999</v>
+        <v>15.5989</v>
       </c>
       <c r="W6" s="2">
-        <v>-88.669700000000006</v>
+        <v>-87.208799999999997</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -2129,7 +2129,7 @@
         <v>46</v>
       </c>
       <c r="V7" s="2">
-        <v>14.550800000000001</v>
+        <v>15.599</v>
       </c>
       <c r="W7" s="2">
         <v>-88.659800000000004</v>
@@ -2197,10 +2197,10 @@
         <v>51</v>
       </c>
       <c r="V8" s="2">
-        <v>14.6058</v>
+        <v>15.7738</v>
       </c>
       <c r="W8" s="2">
-        <v>-88.583200000000005</v>
+        <v>-87.475499999999997</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -2265,10 +2265,10 @@
         <v>52</v>
       </c>
       <c r="V9" s="2">
-        <v>14.4788</v>
+        <v>15.7744</v>
       </c>
       <c r="W9" s="2">
-        <v>-88.595200000000006</v>
+        <v>-87.446799999999996</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -2333,10 +2333,10 @@
         <v>53</v>
       </c>
       <c r="V10" s="2">
-        <v>14.4823</v>
+        <v>15.781700000000001</v>
       </c>
       <c r="W10" s="2">
-        <v>-88.591300000000004</v>
+        <v>-87.453400000000002</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -2401,10 +2401,10 @@
         <v>54</v>
       </c>
       <c r="V11" s="2">
-        <v>14.806699999999999</v>
+        <v>15.783300000000001</v>
       </c>
       <c r="W11" s="2">
-        <v>-88.415999999999997</v>
+        <v>-87.452100000000002</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -2469,10 +2469,10 @@
         <v>37</v>
       </c>
       <c r="V12" s="2">
-        <v>14.809799999999999</v>
+        <v>15.7834</v>
       </c>
       <c r="W12" s="2">
-        <v>-88.410499999999999</v>
+        <v>-87.449399999999997</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -2537,10 +2537,10 @@
         <v>55</v>
       </c>
       <c r="V13" s="2">
-        <v>14.8119</v>
+        <v>15.783899999999999</v>
       </c>
       <c r="W13" s="2">
-        <v>-88.41</v>
+        <v>-87.449700000000007</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -2605,10 +2605,10 @@
         <v>37</v>
       </c>
       <c r="V14" s="2">
-        <v>14.8123</v>
+        <v>15.7841</v>
       </c>
       <c r="W14" s="2">
-        <v>-88.409099999999995</v>
+        <v>-87.450699999999998</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -2673,10 +2673,10 @@
         <v>56</v>
       </c>
       <c r="V15" s="2">
-        <v>14.8123</v>
+        <v>15.7845</v>
       </c>
       <c r="W15" s="2">
-        <v>-88.411100000000005</v>
+        <v>-87.451599999999999</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -2741,10 +2741,10 @@
         <v>62</v>
       </c>
       <c r="V16" s="2">
-        <v>14.8126</v>
+        <v>14.447100000000001</v>
       </c>
       <c r="W16" s="2">
-        <v>-88.408600000000007</v>
+        <v>-87.633300000000006</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -2809,10 +2809,10 @@
         <v>36</v>
       </c>
       <c r="V17" s="2">
-        <v>14.8131</v>
+        <v>14.4542</v>
       </c>
       <c r="W17" s="2">
-        <v>-88.410700000000006</v>
+        <v>-87.643900000000002</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -2877,10 +2877,10 @@
         <v>62</v>
       </c>
       <c r="V18" s="2">
-        <v>14.813499999999999</v>
+        <v>14.454499999999999</v>
       </c>
       <c r="W18" s="2">
-        <v>-88.409599999999998</v>
+        <v>-87.643500000000003</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -2945,10 +2945,10 @@
         <v>63</v>
       </c>
       <c r="V19" s="2">
-        <v>14.8431</v>
+        <v>14.4549</v>
       </c>
       <c r="W19" s="2">
-        <v>-88.456699999999998</v>
+        <v>-87.639200000000002</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -3013,10 +3013,10 @@
         <v>64</v>
       </c>
       <c r="V20" s="2">
-        <v>14.8437</v>
+        <v>14.4573</v>
       </c>
       <c r="W20" s="2">
-        <v>-88.458200000000005</v>
+        <v>-87.642300000000006</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -3081,10 +3081,10 @@
         <v>64</v>
       </c>
       <c r="V21" s="2">
-        <v>14.0588</v>
+        <v>14.458</v>
       </c>
       <c r="W21" s="2">
-        <v>-88.6922</v>
+        <v>-87.640900000000002</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -3149,10 +3149,10 @@
         <v>37</v>
       </c>
       <c r="V22" s="2">
-        <v>14.7813</v>
+        <v>14.596399999999999</v>
       </c>
       <c r="W22" s="2">
-        <v>-88.585999999999999</v>
+        <v>-87.831199999999995</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -3217,10 +3217,10 @@
         <v>69</v>
       </c>
       <c r="V23" s="2">
-        <v>14.599460000000001</v>
+        <v>14.596500000000001</v>
       </c>
       <c r="W23" s="2">
-        <v>-87.843118000000004</v>
+        <v>-87.832300000000004</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -3285,10 +3285,10 @@
         <v>37</v>
       </c>
       <c r="V24" s="2">
-        <v>14.433299999999999</v>
+        <v>14.598699999999999</v>
       </c>
       <c r="W24" s="2">
-        <v>-89.182699999999997</v>
+        <v>-87.831400000000002</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -3353,10 +3353,10 @@
         <v>51</v>
       </c>
       <c r="V25" s="2">
-        <v>14.4337</v>
+        <v>14.767799999999999</v>
       </c>
       <c r="W25" s="2">
-        <v>-89.180400000000006</v>
+        <v>-88.779300000000006</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -3421,10 +3421,10 @@
         <v>62</v>
       </c>
       <c r="V26" s="2">
-        <v>14.433999999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W26" s="2">
-        <v>-89.183000000000007</v>
+        <v>-88.777600000000007</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -3489,10 +3489,10 @@
         <v>62</v>
       </c>
       <c r="V27" s="2">
-        <v>14.434699999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W27" s="2">
-        <v>-89.183300000000003</v>
+        <v>-88.777500000000003</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -3557,10 +3557,10 @@
         <v>80</v>
       </c>
       <c r="V28" s="2">
-        <v>14.434699999999999</v>
+        <v>14.832100000000001</v>
       </c>
       <c r="W28" s="2">
-        <v>-89.183000000000007</v>
+        <v>-89094</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -3625,10 +3625,10 @@
         <v>85</v>
       </c>
       <c r="V29" s="2">
-        <v>14.4351</v>
+        <v>14.8384</v>
       </c>
       <c r="W29" s="2">
-        <v>-89.183700000000002</v>
+        <v>-89.1554</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -3693,10 +3693,10 @@
         <v>36</v>
       </c>
       <c r="V30" s="2">
-        <v>14.4352</v>
+        <v>15.065799999999999</v>
       </c>
       <c r="W30" s="2">
-        <v>-89.182699999999997</v>
+        <v>-88.747100000000003</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -3761,10 +3761,10 @@
         <v>37</v>
       </c>
       <c r="V31" s="2">
-        <v>14.4352</v>
+        <v>15.477399999999999</v>
       </c>
       <c r="W31" s="2">
-        <v>-89.182000000000002</v>
+        <v>-87.985699999999994</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -3829,10 +3829,10 @@
         <v>62</v>
       </c>
       <c r="V32" s="2">
-        <v>14.4354</v>
+        <v>15.4787</v>
       </c>
       <c r="W32" s="2">
-        <v>-89.183000000000007</v>
+        <v>-87.975099999999998</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -3897,10 +3897,10 @@
         <v>97</v>
       </c>
       <c r="V33" s="2">
-        <v>14.435600000000001</v>
+        <v>15.4796</v>
       </c>
       <c r="W33" s="2">
-        <v>-89.182100000000005</v>
+        <v>-88.011200000000002</v>
       </c>
     </row>
     <row r="34" spans="1:23">
@@ -3965,10 +3965,10 @@
         <v>55</v>
       </c>
       <c r="V34" s="2">
-        <v>14.435600000000001</v>
+        <v>15.4854</v>
       </c>
       <c r="W34" s="2">
-        <v>-89.183599999999998</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="35" spans="1:23">
@@ -4033,10 +4033,10 @@
         <v>98</v>
       </c>
       <c r="V35" s="2">
-        <v>14.436</v>
+        <v>15.4855</v>
       </c>
       <c r="W35" s="2">
-        <v>-89.182100000000005</v>
+        <v>-87.984399999999994</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -4101,10 +4101,10 @@
         <v>99</v>
       </c>
       <c r="V36" s="2">
-        <v>14.436299999999999</v>
+        <v>15.489800000000001</v>
       </c>
       <c r="W36" s="2">
-        <v>-89.182299999999998</v>
+        <v>-87.986000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:23">
@@ -4169,10 +4169,10 @@
         <v>100</v>
       </c>
       <c r="V37" s="2">
-        <v>14.4368</v>
+        <v>15.492599999999999</v>
       </c>
       <c r="W37" s="2">
-        <v>-89.182900000000004</v>
+        <v>-88.011499999999998</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -4237,10 +4237,10 @@
         <v>37</v>
       </c>
       <c r="V38" s="2">
-        <v>14.4369</v>
+        <v>15.492699999999999</v>
       </c>
       <c r="W38" s="2">
-        <v>-89.182900000000004</v>
+        <v>-88.016499999999994</v>
       </c>
     </row>
     <row r="39" spans="1:23">
@@ -4305,10 +4305,10 @@
         <v>37</v>
       </c>
       <c r="V39" s="2">
-        <v>14.4369</v>
+        <v>15.4933</v>
       </c>
       <c r="W39" s="2">
-        <v>-89.1828</v>
+        <v>-87.986500000000007</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -4373,10 +4373,10 @@
         <v>37</v>
       </c>
       <c r="V40" s="2">
-        <v>14.437099999999999</v>
+        <v>15.493399999999999</v>
       </c>
       <c r="W40" s="2">
-        <v>-89.182400000000001</v>
+        <v>-87.984800000000007</v>
       </c>
     </row>
     <row r="41" spans="1:23">
@@ -4441,10 +4441,10 @@
         <v>37</v>
       </c>
       <c r="V41" s="2">
-        <v>14.438000000000001</v>
+        <v>15.493600000000001</v>
       </c>
       <c r="W41" s="2">
-        <v>-89.182299999999998</v>
+        <v>-87.984099999999998</v>
       </c>
     </row>
     <row r="42" spans="1:23">
@@ -4509,10 +4509,10 @@
         <v>36</v>
       </c>
       <c r="V42" s="2">
-        <v>14.438000000000001</v>
+        <v>15.494300000000001</v>
       </c>
       <c r="W42" s="2">
-        <v>-89.182100000000005</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="43" spans="1:23">
@@ -4577,10 +4577,10 @@
         <v>101</v>
       </c>
       <c r="V43" s="2">
-        <v>14.438499999999999</v>
+        <v>15.499700000000001</v>
       </c>
       <c r="W43" s="2">
-        <v>-89.183300000000003</v>
+        <v>-88.025000000000006</v>
       </c>
     </row>
     <row r="44" spans="1:23">
@@ -4645,10 +4645,10 @@
         <v>102</v>
       </c>
       <c r="V44" s="2">
-        <v>14.3742</v>
+        <v>15.4999</v>
       </c>
       <c r="W44" s="2">
-        <v>-89.209400000000002</v>
+        <v>-88.037499999999994</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -4713,10 +4713,10 @@
         <v>103</v>
       </c>
       <c r="V45" s="2">
-        <v>14.3748</v>
+        <v>15.5</v>
       </c>
       <c r="W45" s="2">
-        <v>-89.209299999999999</v>
+        <v>-88.020700000000005</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -4781,10 +4781,10 @@
         <v>37</v>
       </c>
       <c r="V46" s="2">
-        <v>14.3749</v>
+        <v>15.500299999999999</v>
       </c>
       <c r="W46" s="2">
-        <v>-89.209400000000002</v>
+        <v>-88.038399999999996</v>
       </c>
     </row>
     <row r="47" spans="1:23">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2020 22-21-49
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46D35F55-0837-4980-95C8-1F5934711C2F}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8B2D6D9-C32C-402A-8733-2A999E79A4F3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="S34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD47"/>
+      <pane ySplit="1" topLeftCell="S55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -4849,10 +4849,10 @@
         <v>104</v>
       </c>
       <c r="V47" s="2">
-        <v>14.3788</v>
+        <v>15.501799999999999</v>
       </c>
       <c r="W47" s="2">
-        <v>-89.128399999999999</v>
+        <v>-88.027100000000004</v>
       </c>
     </row>
     <row r="48" spans="1:23">
@@ -4917,10 +4917,10 @@
         <v>62</v>
       </c>
       <c r="V48" s="2">
-        <v>14.380699999999999</v>
+        <v>15.504099999999999</v>
       </c>
       <c r="W48" s="2">
-        <v>-89.130899999999997</v>
+        <v>-88.014200000000002</v>
       </c>
     </row>
     <row r="49" spans="1:23">
@@ -4985,10 +4985,10 @@
         <v>105</v>
       </c>
       <c r="V49" s="2">
-        <v>14.4985</v>
+        <v>15.505100000000001</v>
       </c>
       <c r="W49" s="2">
-        <v>-88.753500000000003</v>
+        <v>-88.022300000000001</v>
       </c>
     </row>
     <row r="50" spans="1:23">
@@ -5053,10 +5053,10 @@
         <v>106</v>
       </c>
       <c r="V50" s="2">
-        <v>14.5349</v>
+        <v>15.5061</v>
       </c>
       <c r="W50" s="2">
-        <v>-89.279399999999995</v>
+        <v>-88.027199999999993</v>
       </c>
     </row>
     <row r="51" spans="1:23">
@@ -5121,10 +5121,10 @@
         <v>63</v>
       </c>
       <c r="V51" s="2">
-        <v>14.4854</v>
+        <v>15.5105</v>
       </c>
       <c r="W51" s="2">
-        <v>-88.978999999999999</v>
+        <v>-88.012699999999995</v>
       </c>
     </row>
     <row r="52" spans="1:23">
@@ -5189,10 +5189,10 @@
         <v>37</v>
       </c>
       <c r="V52" s="2">
-        <v>14.658099999999999</v>
+        <v>15.5124</v>
       </c>
       <c r="W52" s="2">
-        <v>-86.214799999999997</v>
+        <v>-88.037000000000006</v>
       </c>
     </row>
     <row r="53" spans="1:23">
@@ -5257,10 +5257,10 @@
         <v>62</v>
       </c>
       <c r="V53" s="2">
-        <v>14.662800000000001</v>
+        <v>15.5146</v>
       </c>
       <c r="W53" s="2">
-        <v>-86.216300000000004</v>
+        <v>-88.033600000000007</v>
       </c>
     </row>
     <row r="54" spans="1:23">
@@ -5325,10 +5325,10 @@
         <v>37</v>
       </c>
       <c r="V54" s="2">
-        <v>14.664300000000001</v>
+        <v>15.5159</v>
       </c>
       <c r="W54" s="2">
-        <v>-86.2166</v>
+        <v>-88.028400000000005</v>
       </c>
     </row>
     <row r="55" spans="1:23">
@@ -5393,10 +5393,10 @@
         <v>36</v>
       </c>
       <c r="V55" s="2">
-        <v>14.664300000000001</v>
+        <v>15.5244</v>
       </c>
       <c r="W55" s="2">
-        <v>-86.216300000000004</v>
+        <v>-88.038499999999999</v>
       </c>
     </row>
     <row r="56" spans="1:23">
@@ -5461,10 +5461,10 @@
         <v>107</v>
       </c>
       <c r="V56" s="2">
-        <v>14.664999999999999</v>
+        <v>15.5298</v>
       </c>
       <c r="W56" s="2">
-        <v>-86.215699999999998</v>
+        <v>-88.032700000000006</v>
       </c>
     </row>
     <row r="57" spans="1:23">
@@ -5529,10 +5529,10 @@
         <v>37</v>
       </c>
       <c r="V57" s="2">
-        <v>14.670400000000001</v>
+        <v>15.5299</v>
       </c>
       <c r="W57" s="2">
-        <v>-86.218900000000005</v>
+        <v>-88.026499999999999</v>
       </c>
     </row>
     <row r="58" spans="1:23">
@@ -5597,10 +5597,10 @@
         <v>36</v>
       </c>
       <c r="V58" s="2">
-        <v>14.6706</v>
+        <v>15.5299</v>
       </c>
       <c r="W58" s="2">
-        <v>-86.222300000000004</v>
+        <v>-88.025499999999994</v>
       </c>
     </row>
     <row r="59" spans="1:23">
@@ -5665,10 +5665,10 @@
         <v>36</v>
       </c>
       <c r="V59" s="2">
-        <v>14.6706</v>
+        <v>15.5306</v>
       </c>
       <c r="W59" s="2">
-        <v>-86.221199999999996</v>
+        <v>-88.029399999999995</v>
       </c>
     </row>
     <row r="60" spans="1:23">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-20-2020 01-22-08
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="265" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8B2D6D9-C32C-402A-8733-2A999E79A4F3}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{47431B76-5D7D-42F3-A95B-4B9BBE5452D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="S55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60:XFD60"/>
+      <pane ySplit="1" topLeftCell="S126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132:XFD132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -5733,10 +5733,10 @@
         <v>37</v>
       </c>
       <c r="V60" s="2">
-        <v>14.6767</v>
+        <v>15.5341</v>
       </c>
       <c r="W60" s="2">
-        <v>-86.205299999999994</v>
+        <v>-88.019300000000001</v>
       </c>
     </row>
     <row r="61" spans="1:23">
@@ -5801,10 +5801,10 @@
         <v>36</v>
       </c>
       <c r="V61" s="2">
-        <v>14.7057</v>
+        <v>15.537100000000001</v>
       </c>
       <c r="W61" s="2">
-        <v>-86.167599999999993</v>
+        <v>-88.014899999999997</v>
       </c>
     </row>
     <row r="62" spans="1:23">
@@ -5869,10 +5869,10 @@
         <v>37</v>
       </c>
       <c r="V62" s="2">
-        <v>14.6373</v>
+        <v>15.542899999999999</v>
       </c>
       <c r="W62" s="2">
-        <v>-86.219200000000001</v>
+        <v>-88.023099999999999</v>
       </c>
     </row>
     <row r="63" spans="1:23">
@@ -5937,10 +5937,10 @@
         <v>37</v>
       </c>
       <c r="V63" s="2">
-        <v>14.7018</v>
+        <v>15.549099999999999</v>
       </c>
       <c r="W63" s="2">
-        <v>-86.034400000000005</v>
+        <v>-88.035899999999998</v>
       </c>
     </row>
     <row r="64" spans="1:23">
@@ -6005,10 +6005,10 @@
         <v>37</v>
       </c>
       <c r="V64" s="2">
-        <v>14.7232</v>
+        <v>15.5505</v>
       </c>
       <c r="W64" s="2">
-        <v>-86.138099999999994</v>
+        <v>-88.004800000000003</v>
       </c>
     </row>
     <row r="65" spans="1:23">
@@ -6073,10 +6073,10 @@
         <v>62</v>
       </c>
       <c r="V65" s="2">
-        <v>14.8385</v>
+        <v>15.6119</v>
       </c>
       <c r="W65" s="2">
-        <v>-85.882800000000003</v>
+        <v>-87.956299999999999</v>
       </c>
     </row>
     <row r="66" spans="1:23">
@@ -6141,10 +6141,10 @@
         <v>62</v>
       </c>
       <c r="V66" s="2">
-        <v>14.840999999999999</v>
+        <v>15.316800000000001</v>
       </c>
       <c r="W66" s="2">
-        <v>-85.904200000000003</v>
+        <v>-87.990300000000005</v>
       </c>
     </row>
     <row r="67" spans="1:23">
@@ -6209,10 +6209,10 @@
         <v>37</v>
       </c>
       <c r="V67" s="2">
-        <v>14.8454</v>
+        <v>15.4361</v>
       </c>
       <c r="W67" s="2">
-        <v>-85.900700000000001</v>
+        <v>-87.921099999999996</v>
       </c>
     </row>
     <row r="68" spans="1:23">
@@ -6277,10 +6277,10 @@
         <v>62</v>
       </c>
       <c r="V68" s="2">
-        <v>15.083600000000001</v>
+        <v>15.436500000000001</v>
       </c>
       <c r="W68" s="2">
-        <v>-85.558899999999994</v>
+        <v>-87.924300000000002</v>
       </c>
     </row>
     <row r="69" spans="1:23">
@@ -6345,10 +6345,10 @@
         <v>37</v>
       </c>
       <c r="V69" s="2">
-        <v>15.0847</v>
+        <v>15.438499999999999</v>
       </c>
       <c r="W69" s="2">
-        <v>-85.557900000000004</v>
+        <v>-87.926900000000003</v>
       </c>
     </row>
     <row r="70" spans="1:23">
@@ -6413,10 +6413,10 @@
         <v>120</v>
       </c>
       <c r="V70" s="2">
-        <v>15.030799999999999</v>
+        <v>15.4405</v>
       </c>
       <c r="W70" s="2">
-        <v>-86.068600000000004</v>
+        <v>-87.929100000000005</v>
       </c>
     </row>
     <row r="71" spans="1:23">
@@ -6481,10 +6481,10 @@
         <v>37</v>
       </c>
       <c r="V71" s="2">
-        <v>15.5166</v>
+        <v>13.309900000000001</v>
       </c>
       <c r="W71" s="2">
-        <v>-85.866600000000005</v>
+        <v>-87.179100000000005</v>
       </c>
     </row>
     <row r="72" spans="1:23">
@@ -6549,10 +6549,10 @@
         <v>37</v>
       </c>
       <c r="V72" s="2">
-        <v>15.518599999999999</v>
+        <v>13.3125</v>
       </c>
       <c r="W72" s="2">
-        <v>-85.873000000000005</v>
+        <v>-87.175299999999993</v>
       </c>
     </row>
     <row r="73" spans="1:23">
@@ -6617,10 +6617,10 @@
         <v>131</v>
       </c>
       <c r="V73" s="2">
-        <v>15.198499999999999</v>
+        <v>13.095800000000001</v>
       </c>
       <c r="W73" s="2">
-        <v>-85.772199999999998</v>
+        <v>-87.057100000000005</v>
       </c>
     </row>
     <row r="74" spans="1:23">
@@ -6685,10 +6685,10 @@
         <v>36</v>
       </c>
       <c r="V74" s="2">
-        <v>15.259399999999999</v>
+        <v>14.0412</v>
       </c>
       <c r="W74" s="2">
-        <v>-85.746200000000002</v>
+        <v>-87.232399999999998</v>
       </c>
     </row>
     <row r="75" spans="1:23">
@@ -6753,10 +6753,10 @@
         <v>55</v>
       </c>
       <c r="V75" s="2">
-        <v>14.869400000000001</v>
+        <v>14.0457</v>
       </c>
       <c r="W75" s="2">
-        <v>-86.183800000000005</v>
+        <v>-87.211399999999998</v>
       </c>
     </row>
     <row r="76" spans="1:23">
@@ -6821,10 +6821,10 @@
         <v>36</v>
       </c>
       <c r="V76" s="2">
-        <v>14.351000000000001</v>
+        <v>14.0543</v>
       </c>
       <c r="W76" s="2">
-        <v>-85.887799999999999</v>
+        <v>-87.2226</v>
       </c>
     </row>
     <row r="77" spans="1:23">
@@ -6889,10 +6889,10 @@
         <v>106</v>
       </c>
       <c r="V77" s="2">
-        <v>14.9177</v>
+        <v>14.055099999999999</v>
       </c>
       <c r="W77" s="2">
-        <v>-88.237200000000001</v>
+        <v>-87.222300000000004</v>
       </c>
     </row>
     <row r="78" spans="1:23">
@@ -6957,10 +6957,10 @@
         <v>107</v>
       </c>
       <c r="V78" s="2">
-        <v>14.920199999999999</v>
+        <v>14.055400000000001</v>
       </c>
       <c r="W78" s="2">
-        <v>-88.245099999999994</v>
+        <v>-87.222099999999998</v>
       </c>
     </row>
     <row r="79" spans="1:23">
@@ -7025,10 +7025,10 @@
         <v>37</v>
       </c>
       <c r="V79" s="2">
-        <v>14.9216</v>
+        <v>14.0558</v>
       </c>
       <c r="W79" s="2">
-        <v>-88.237200000000001</v>
+        <v>-87.229299999999995</v>
       </c>
     </row>
     <row r="80" spans="1:23">
@@ -7093,10 +7093,10 @@
         <v>138</v>
       </c>
       <c r="V80" s="2">
-        <v>14.923299999999999</v>
+        <v>14.0588</v>
       </c>
       <c r="W80" s="2">
-        <v>-88.244500000000002</v>
+        <v>-87.189599999999999</v>
       </c>
     </row>
     <row r="81" spans="1:23">
@@ -7161,10 +7161,10 @@
         <v>106</v>
       </c>
       <c r="V81" s="2">
-        <v>14.927899999999999</v>
+        <v>14.058999999999999</v>
       </c>
       <c r="W81" s="2">
-        <v>-88.236900000000006</v>
+        <v>-87.189400000000006</v>
       </c>
     </row>
     <row r="82" spans="1:23">
@@ -7229,10 +7229,10 @@
         <v>139</v>
       </c>
       <c r="V82" s="2">
-        <v>14.8439</v>
+        <v>14.059100000000001</v>
       </c>
       <c r="W82" s="2">
-        <v>-88.461799999999997</v>
+        <v>-87.220600000000005</v>
       </c>
     </row>
     <row r="83" spans="1:23">
@@ -7297,10 +7297,10 @@
         <v>36</v>
       </c>
       <c r="V83" s="2">
-        <v>15.2621</v>
+        <v>14.0601</v>
       </c>
       <c r="W83" s="2">
-        <v>-88.541700000000006</v>
+        <v>-83.400400000000005</v>
       </c>
     </row>
     <row r="84" spans="1:23">
@@ -7365,10 +7365,10 @@
         <v>140</v>
       </c>
       <c r="V84" s="2">
-        <v>15.2738</v>
+        <v>14.064</v>
       </c>
       <c r="W84" s="2">
-        <v>-88.282899999999998</v>
+        <v>-87.209599999999995</v>
       </c>
     </row>
     <row r="85" spans="1:23">
@@ -7433,10 +7433,10 @@
         <v>37</v>
       </c>
       <c r="V85" s="2">
-        <v>15.3117</v>
+        <v>14.0655</v>
       </c>
       <c r="W85" s="2">
-        <v>-88.439599999999999</v>
+        <v>-87.1785</v>
       </c>
     </row>
     <row r="86" spans="1:23">
@@ -7501,10 +7501,10 @@
         <v>107</v>
       </c>
       <c r="V86" s="2">
-        <v>15.3123</v>
+        <v>14.0655</v>
       </c>
       <c r="W86" s="2">
-        <v>-88.439700000000002</v>
+        <v>-87.179299999999998</v>
       </c>
     </row>
     <row r="87" spans="1:23">
@@ -7569,10 +7569,10 @@
         <v>107</v>
       </c>
       <c r="V87" s="2">
-        <v>15.3133</v>
+        <v>14.0655</v>
       </c>
       <c r="W87" s="2">
-        <v>-88.436899999999994</v>
+        <v>-87.179599999999994</v>
       </c>
     </row>
     <row r="88" spans="1:23">
@@ -7637,10 +7637,10 @@
         <v>141</v>
       </c>
       <c r="V88" s="2">
-        <v>15.314</v>
+        <v>14.0665</v>
       </c>
       <c r="W88" s="2">
-        <v>-88.440200000000004</v>
+        <v>-87.210700000000003</v>
       </c>
     </row>
     <row r="89" spans="1:23">
@@ -7705,10 +7705,10 @@
         <v>106</v>
       </c>
       <c r="V89" s="2">
-        <v>15.314299999999999</v>
+        <v>14.0692</v>
       </c>
       <c r="W89" s="2">
-        <v>-88.437200000000004</v>
+        <v>-87.185000000000002</v>
       </c>
     </row>
     <row r="90" spans="1:23">
@@ -7773,10 +7773,10 @@
         <v>37</v>
       </c>
       <c r="V90" s="2">
-        <v>15.371499999999999</v>
+        <v>14.081799999999999</v>
       </c>
       <c r="W90" s="2">
-        <v>-88.299599999999998</v>
+        <v>-87.209599999999995</v>
       </c>
     </row>
     <row r="91" spans="1:23">
@@ -7841,10 +7841,10 @@
         <v>106</v>
       </c>
       <c r="V91" s="2">
-        <v>14.8527</v>
+        <v>14.083399999999999</v>
       </c>
       <c r="W91" s="2">
-        <v>-88.419799999999995</v>
+        <v>-87.174999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:23">
@@ -7909,10 +7909,10 @@
         <v>36</v>
       </c>
       <c r="V92" s="2">
-        <v>14.7552</v>
+        <v>14.0837</v>
       </c>
       <c r="W92" s="2">
-        <v>-88.114400000000003</v>
+        <v>-87.210099999999997</v>
       </c>
     </row>
     <row r="93" spans="1:23">
@@ -7977,10 +7977,10 @@
         <v>36</v>
       </c>
       <c r="V93" s="2">
-        <v>14.769399999999999</v>
+        <v>14.0844</v>
       </c>
       <c r="W93" s="2">
-        <v>-88.145799999999994</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="94" spans="1:23">
@@ -8045,10 +8045,10 @@
         <v>37</v>
       </c>
       <c r="V94" s="2">
-        <v>15.1439</v>
+        <v>14.085000000000001</v>
       </c>
       <c r="W94" s="2">
-        <v>-88.234700000000004</v>
+        <v>-87.186999999999998</v>
       </c>
     </row>
     <row r="95" spans="1:23">
@@ -8113,10 +8113,10 @@
         <v>62</v>
       </c>
       <c r="V95" s="2">
-        <v>14.8727</v>
+        <v>14.085900000000001</v>
       </c>
       <c r="W95" s="2">
-        <v>-88.072199999999995</v>
+        <v>-87.174400000000006</v>
       </c>
     </row>
     <row r="96" spans="1:23">
@@ -8181,10 +8181,10 @@
         <v>51</v>
       </c>
       <c r="V96" s="2">
-        <v>13.5328</v>
+        <v>14.0869</v>
       </c>
       <c r="W96" s="2">
-        <v>-87.552300000000002</v>
+        <v>-87.184899999999999</v>
       </c>
     </row>
     <row r="97" spans="1:23">
@@ -8249,10 +8249,10 @@
         <v>36</v>
       </c>
       <c r="V97" s="2">
-        <v>13.378299999999999</v>
+        <v>14.088200000000001</v>
       </c>
       <c r="W97" s="2">
-        <v>-87.575900000000004</v>
+        <v>-87.183400000000006</v>
       </c>
     </row>
     <row r="98" spans="1:23">
@@ -8317,10 +8317,10 @@
         <v>36</v>
       </c>
       <c r="V98" s="2">
-        <v>13.4994</v>
+        <v>14.089600000000001</v>
       </c>
       <c r="W98" s="2">
-        <v>-87.442599999999999</v>
+        <v>-87.188500000000005</v>
       </c>
     </row>
     <row r="99" spans="1:23">
@@ -8385,10 +8385,10 @@
         <v>37</v>
       </c>
       <c r="V99" s="2">
-        <v>13.5281</v>
+        <v>14.09</v>
       </c>
       <c r="W99" s="2">
-        <v>-87.490200000000002</v>
+        <v>-87.206500000000005</v>
       </c>
     </row>
     <row r="100" spans="1:23">
@@ -8453,10 +8453,10 @@
         <v>106</v>
       </c>
       <c r="V100" s="2">
-        <v>13.532400000000001</v>
+        <v>14.090199999999999</v>
       </c>
       <c r="W100" s="2">
-        <v>-87.501300000000001</v>
+        <v>-87.197199999999995</v>
       </c>
     </row>
     <row r="101" spans="1:23">
@@ -8521,10 +8521,10 @@
         <v>142</v>
       </c>
       <c r="V101" s="2">
-        <v>13.5337</v>
+        <v>14.090400000000001</v>
       </c>
       <c r="W101" s="2">
-        <v>-87.496300000000005</v>
+        <v>-87.196799999999996</v>
       </c>
     </row>
     <row r="102" spans="1:23">
@@ -8589,10 +8589,10 @@
         <v>143</v>
       </c>
       <c r="V102" s="2">
-        <v>13.280799999999999</v>
+        <v>14.092599999999999</v>
       </c>
       <c r="W102" s="2">
-        <v>-87.655299999999997</v>
+        <v>-87.2393</v>
       </c>
     </row>
     <row r="103" spans="1:23">
@@ -8657,10 +8657,10 @@
         <v>143</v>
       </c>
       <c r="V103" s="2">
-        <v>13.2742</v>
+        <v>14.092700000000001</v>
       </c>
       <c r="W103" s="2">
-        <v>-87.613799999999998</v>
+        <v>-87.194100000000006</v>
       </c>
     </row>
     <row r="104" spans="1:23">
@@ -8725,10 +8725,10 @@
         <v>143</v>
       </c>
       <c r="V104" s="2">
-        <v>13.285</v>
+        <v>14.0928</v>
       </c>
       <c r="W104" s="2">
-        <v>-87.621499999999997</v>
+        <v>-87.218500000000006</v>
       </c>
     </row>
     <row r="105" spans="1:23">
@@ -8793,10 +8793,10 @@
         <v>144</v>
       </c>
       <c r="V105" s="2">
-        <v>13.3597</v>
+        <v>14.0947</v>
       </c>
       <c r="W105" s="2">
-        <v>-87.599599999999995</v>
+        <v>-87.1952</v>
       </c>
     </row>
     <row r="106" spans="1:23">
@@ -8861,10 +8861,10 @@
         <v>62</v>
       </c>
       <c r="V106" s="2">
-        <v>13.2681</v>
+        <v>14.095700000000001</v>
       </c>
       <c r="W106" s="2">
-        <v>-87.658199999999994</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="107" spans="1:23">
@@ -8929,10 +8929,10 @@
         <v>145</v>
       </c>
       <c r="V107" s="2">
-        <v>13.268700000000001</v>
+        <v>14.095700000000001</v>
       </c>
       <c r="W107" s="2">
-        <v>-87.657600000000002</v>
+        <v>-87.211200000000005</v>
       </c>
     </row>
     <row r="108" spans="1:23">
@@ -8997,10 +8997,10 @@
         <v>146</v>
       </c>
       <c r="V108" s="2">
-        <v>13.251200000000001</v>
+        <v>14.097</v>
       </c>
       <c r="W108" s="2">
-        <v>-87.6511</v>
+        <v>-87.207499999999996</v>
       </c>
     </row>
     <row r="109" spans="1:23">
@@ -9065,10 +9065,10 @@
         <v>147</v>
       </c>
       <c r="V109" s="2">
-        <v>13.254</v>
+        <v>14.097</v>
       </c>
       <c r="W109" s="2">
-        <v>-87.649000000000001</v>
+        <v>-87.222499999999997</v>
       </c>
     </row>
     <row r="110" spans="1:23">
@@ -9133,10 +9133,10 @@
         <v>37</v>
       </c>
       <c r="V110" s="2">
-        <v>13.595599999999999</v>
+        <v>14.099600000000001</v>
       </c>
       <c r="W110" s="2">
-        <v>-87.761899999999997</v>
+        <v>-87.194500000000005</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -9201,10 +9201,10 @@
         <v>51</v>
       </c>
       <c r="V111" s="2">
-        <v>13.5961</v>
+        <v>14.0998</v>
       </c>
       <c r="W111" s="2">
-        <v>-87.764600000000002</v>
+        <v>-87.189599999999999</v>
       </c>
     </row>
     <row r="112" spans="1:23">
@@ -9269,10 +9269,10 @@
         <v>36</v>
       </c>
       <c r="V112" s="2">
-        <v>13.5962</v>
+        <v>14.0999</v>
       </c>
       <c r="W112" s="2">
-        <v>-87.764700000000005</v>
+        <v>-87.187100000000001</v>
       </c>
     </row>
     <row r="113" spans="1:23">
@@ -9337,10 +9337,10 @@
         <v>107</v>
       </c>
       <c r="V113" s="2">
-        <v>13.596299999999999</v>
+        <v>14.1004</v>
       </c>
       <c r="W113" s="2">
-        <v>-87.763400000000004</v>
+        <v>-87.208500000000001</v>
       </c>
     </row>
     <row r="114" spans="1:23">
@@ -9405,10 +9405,10 @@
         <v>37</v>
       </c>
       <c r="V114" s="2">
-        <v>13.593</v>
+        <v>14.1004</v>
       </c>
       <c r="W114" s="2">
-        <v>-87.750600000000006</v>
+        <v>-87.183999999999997</v>
       </c>
     </row>
     <row r="115" spans="1:23">
@@ -9473,10 +9473,10 @@
         <v>107</v>
       </c>
       <c r="V115" s="2">
-        <v>13.4175</v>
+        <v>14.1006</v>
       </c>
       <c r="W115" s="2">
-        <v>-87.448099999999997</v>
+        <v>-87.182199999999995</v>
       </c>
     </row>
     <row r="116" spans="1:23">
@@ -9541,10 +9541,10 @@
         <v>36</v>
       </c>
       <c r="V116" s="2">
-        <v>13.4191</v>
+        <v>14.1007</v>
       </c>
       <c r="W116" s="2">
-        <v>-87.448300000000003</v>
+        <v>-87.180599999999998</v>
       </c>
     </row>
     <row r="117" spans="1:23">
@@ -9609,10 +9609,10 @@
         <v>106</v>
       </c>
       <c r="V117" s="2">
-        <v>13.4306</v>
+        <v>14.1007</v>
       </c>
       <c r="W117" s="2">
-        <v>-87.4285</v>
+        <v>-87.183400000000006</v>
       </c>
     </row>
     <row r="118" spans="1:23">
@@ -9677,10 +9677,10 @@
         <v>148</v>
       </c>
       <c r="V118" s="2">
-        <v>13.4314</v>
+        <v>14.101000000000001</v>
       </c>
       <c r="W118" s="2">
-        <v>-87.449700000000007</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="119" spans="1:23">
@@ -9745,10 +9745,10 @@
         <v>149</v>
       </c>
       <c r="V119" s="2">
-        <v>13.4329</v>
+        <v>14.1014</v>
       </c>
       <c r="W119" s="2">
-        <v>-87.450699999999998</v>
+        <v>-87.207800000000006</v>
       </c>
     </row>
     <row r="120" spans="1:23">
@@ -9813,10 +9813,10 @@
         <v>36</v>
       </c>
       <c r="V120" s="2">
-        <v>13.434200000000001</v>
+        <v>14.102600000000001</v>
       </c>
       <c r="W120" s="2">
-        <v>-87.427700000000002</v>
+        <v>-87.184799999999996</v>
       </c>
     </row>
     <row r="121" spans="1:23">
@@ -9881,10 +9881,10 @@
         <v>37</v>
       </c>
       <c r="V121" s="2">
-        <v>13.436299999999999</v>
+        <v>14.1028</v>
       </c>
       <c r="W121" s="2">
-        <v>-87.4512</v>
+        <v>-87.178899999999999</v>
       </c>
     </row>
     <row r="122" spans="1:23">
@@ -9949,10 +9949,10 @@
         <v>107</v>
       </c>
       <c r="V122" s="2">
-        <v>13.439500000000001</v>
+        <v>14.1029</v>
       </c>
       <c r="W122" s="2">
-        <v>-87.451400000000007</v>
+        <v>-87.196799999999996</v>
       </c>
     </row>
     <row r="123" spans="1:23">
@@ -10017,10 +10017,10 @@
         <v>150</v>
       </c>
       <c r="V123" s="2">
-        <v>13.4544</v>
+        <v>14.1043</v>
       </c>
       <c r="W123" s="2">
-        <v>-87.453800000000001</v>
+        <v>-87.198599999999999</v>
       </c>
     </row>
     <row r="124" spans="1:23">
@@ -10085,10 +10085,10 @@
         <v>37</v>
       </c>
       <c r="V124" s="2">
-        <v>13.4565</v>
+        <v>14.1045</v>
       </c>
       <c r="W124" s="2">
-        <v>-87.453800000000001</v>
+        <v>-87.199200000000005</v>
       </c>
     </row>
     <row r="125" spans="1:23">
@@ -10153,10 +10153,10 @@
         <v>143</v>
       </c>
       <c r="V125" s="2">
-        <v>15.132300000000001</v>
+        <v>14.1046</v>
       </c>
       <c r="W125" s="2">
-        <v>-87.130200000000002</v>
+        <v>-87.236400000000003</v>
       </c>
     </row>
     <row r="126" spans="1:23">
@@ -10221,10 +10221,10 @@
         <v>36</v>
       </c>
       <c r="V126" s="2">
-        <v>15.130599999999999</v>
+        <v>14.1052</v>
       </c>
       <c r="W126" s="2">
-        <v>-87.147199999999998</v>
+        <v>-87.205399999999997</v>
       </c>
     </row>
     <row r="127" spans="1:23">
@@ -10289,10 +10289,10 @@
         <v>37</v>
       </c>
       <c r="V127" s="2">
-        <v>15.5138</v>
+        <v>14.106299999999999</v>
       </c>
       <c r="W127" s="2">
-        <v>-87.6691</v>
+        <v>-87.204499999999996</v>
       </c>
     </row>
     <row r="128" spans="1:23">
@@ -10357,10 +10357,10 @@
         <v>151</v>
       </c>
       <c r="V128" s="2">
-        <v>15.5343</v>
+        <v>14.1065</v>
       </c>
       <c r="W128" s="2">
-        <v>-87.653300000000002</v>
+        <v>-87.205399999999997</v>
       </c>
     </row>
     <row r="129" spans="1:23">
@@ -10425,10 +10425,10 @@
         <v>152</v>
       </c>
       <c r="V129" s="2">
-        <v>15.5352</v>
+        <v>14.1067</v>
       </c>
       <c r="W129" s="2">
-        <v>-87.652600000000007</v>
+        <v>-87.206800000000001</v>
       </c>
     </row>
     <row r="130" spans="1:23">
@@ -10493,10 +10493,10 @@
         <v>153</v>
       </c>
       <c r="V130" s="2">
-        <v>15.536099999999999</v>
+        <v>14.1068</v>
       </c>
       <c r="W130" s="2">
-        <v>-87.653099999999995</v>
+        <v>-87.205799999999996</v>
       </c>
     </row>
     <row r="131" spans="1:23">
@@ -10561,10 +10561,10 @@
         <v>36</v>
       </c>
       <c r="V131" s="2">
-        <v>15.5425</v>
+        <v>14.107900000000001</v>
       </c>
       <c r="W131" s="2">
-        <v>-87.6524</v>
+        <v>-87.205299999999994</v>
       </c>
     </row>
     <row r="132" spans="1:23">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-20-2020 04-22-29
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="410" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{47431B76-5D7D-42F3-A95B-4B9BBE5452D1}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BBFBB4FF-40AE-482C-91A4-7AC0A7377D76}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="203">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -571,9 +571,6 @@
   </si>
   <si>
     <t>HND-1102</t>
-  </si>
-  <si>
-    <t>pharmacy</t>
   </si>
   <si>
     <t>12</t>
@@ -655,7 +652,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,6 +783,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1138,7 +1143,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1147,6 +1152,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1623,11 +1629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W162"/>
+  <dimension ref="A1:AA162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="S126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132:XFD132"/>
+      <pane ySplit="1" topLeftCell="S137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA147" sqref="AA147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -10629,10 +10635,10 @@
         <v>153</v>
       </c>
       <c r="V132" s="2">
-        <v>15.543200000000001</v>
+        <v>14.1082</v>
       </c>
       <c r="W132" s="2">
-        <v>-87.652199999999993</v>
+        <v>-87.2059</v>
       </c>
     </row>
     <row r="133" spans="1:23">
@@ -10697,10 +10703,10 @@
         <v>154</v>
       </c>
       <c r="V133" s="2">
-        <v>15.543200000000001</v>
+        <v>14.1089</v>
       </c>
       <c r="W133" s="2">
-        <v>-87.652199999999993</v>
+        <v>-87.2089</v>
       </c>
     </row>
     <row r="134" spans="1:23">
@@ -10765,10 +10771,10 @@
         <v>107</v>
       </c>
       <c r="V134" s="2">
-        <v>15.543200000000001</v>
+        <v>14.1137</v>
       </c>
       <c r="W134" s="2">
-        <v>-87.652199999999993</v>
+        <v>-87.193799999999996</v>
       </c>
     </row>
     <row r="135" spans="1:23">
@@ -10833,10 +10839,10 @@
         <v>37</v>
       </c>
       <c r="V135" s="2">
-        <v>15.549799999999999</v>
+        <v>14.1287</v>
       </c>
       <c r="W135" s="2">
-        <v>-87.651600000000002</v>
+        <v>-87.227800000000002</v>
       </c>
     </row>
     <row r="136" spans="1:23">
@@ -10901,10 +10907,10 @@
         <v>159</v>
       </c>
       <c r="V136" s="2">
-        <v>15.55</v>
+        <v>14.5402</v>
       </c>
       <c r="W136" s="2">
-        <v>-87.651600000000002</v>
+        <v>-86.831100000000006</v>
       </c>
     </row>
     <row r="137" spans="1:23">
@@ -10969,10 +10975,10 @@
         <v>106</v>
       </c>
       <c r="V137" s="2">
-        <v>15.550800000000001</v>
+        <v>14.541600000000001</v>
       </c>
       <c r="W137" s="2">
-        <v>-87.651399999999995</v>
+        <v>-86.830799999999996</v>
       </c>
     </row>
     <row r="138" spans="1:23">
@@ -11037,10 +11043,10 @@
         <v>55</v>
       </c>
       <c r="V138" s="2">
-        <v>15.552</v>
+        <v>14.5555</v>
       </c>
       <c r="W138" s="2">
-        <v>-87.651300000000006</v>
+        <v>-86.827200000000005</v>
       </c>
     </row>
     <row r="139" spans="1:23">
@@ -11105,10 +11111,10 @@
         <v>55</v>
       </c>
       <c r="V139" s="2">
-        <v>15.3794</v>
+        <v>14.4832</v>
       </c>
       <c r="W139" s="2">
-        <v>-87.807299999999998</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="140" spans="1:23">
@@ -11173,10 +11179,10 @@
         <v>166</v>
       </c>
       <c r="V140" s="2">
-        <v>15.382999999999999</v>
+        <v>14.4839</v>
       </c>
       <c r="W140" s="2">
-        <v>-87.804599999999994</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="141" spans="1:23">
@@ -11241,10 +11247,10 @@
         <v>106</v>
       </c>
       <c r="V141" s="2">
-        <v>15.387600000000001</v>
+        <v>14.4841</v>
       </c>
       <c r="W141" s="2">
-        <v>-87.805400000000006</v>
+        <v>-87.981499999999997</v>
       </c>
     </row>
     <row r="142" spans="1:23">
@@ -11309,10 +11315,10 @@
         <v>55</v>
       </c>
       <c r="V142" s="2">
-        <v>15.3881</v>
+        <v>14.4849</v>
       </c>
       <c r="W142" s="2">
-        <v>-87.811000000000007</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="143" spans="1:23">
@@ -11377,10 +11383,10 @@
         <v>167</v>
       </c>
       <c r="V143" s="2">
-        <v>15.388400000000001</v>
+        <v>14.4855</v>
       </c>
       <c r="W143" s="2">
-        <v>-87.8108</v>
+        <v>-87.981499999999997</v>
       </c>
     </row>
     <row r="144" spans="1:23">
@@ -11445,13 +11451,13 @@
         <v>174</v>
       </c>
       <c r="V144" s="2">
-        <v>15.3889</v>
+        <v>16.319299999999998</v>
       </c>
       <c r="W144" s="2">
-        <v>-87.805899999999994</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23">
+        <v>-86.538700000000006</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27">
       <c r="A145" s="1">
         <v>35879</v>
       </c>
@@ -11510,16 +11516,16 @@
         <v>35</v>
       </c>
       <c r="U145" s="7" t="s">
-        <v>179</v>
+        <v>39</v>
       </c>
       <c r="V145" s="2">
-        <v>15.393000000000001</v>
+        <v>16.442499999999999</v>
       </c>
       <c r="W145" s="2">
-        <v>-87.806200000000004</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23">
+        <v>-85.887699999999995</v>
+      </c>
+    </row>
+    <row r="146" spans="1:27">
       <c r="A146" s="1">
         <v>25855</v>
       </c>
@@ -11536,10 +11542,10 @@
         <v>12</v>
       </c>
       <c r="F146" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G146" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
@@ -11548,10 +11554,10 @@
         <v>17</v>
       </c>
       <c r="J146" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K146" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="K146" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
@@ -11560,16 +11566,16 @@
         <v>7</v>
       </c>
       <c r="N146" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O146" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="O146" s="1" t="s">
+      <c r="P146" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q146" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="P146" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q146" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>34</v>
@@ -11581,13 +11587,13 @@
         <v>39</v>
       </c>
       <c r="V146" s="2">
-        <v>15.393599999999999</v>
+        <v>14.245100000000001</v>
       </c>
       <c r="W146" s="2">
-        <v>-87.807100000000005</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23">
+        <v>-87.898399999999995</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27" ht="15">
       <c r="A147" s="1">
         <v>28037</v>
       </c>
@@ -11604,58 +11610,59 @@
         <v>13</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="H147" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" s="1">
+        <v>1</v>
+      </c>
+      <c r="J147" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I147" s="1">
-        <v>1</v>
-      </c>
-      <c r="J147" s="1" t="s">
+      <c r="K147" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K147" s="1" t="s">
+      <c r="L147" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M147" s="1">
+        <v>1</v>
+      </c>
+      <c r="N147" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L147" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M147" s="1">
-        <v>1</v>
-      </c>
-      <c r="N147" s="1" t="s">
+      <c r="O147" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O147" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q147" s="1" t="s">
+      <c r="R147" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S147" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U147" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="R147" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S147" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U147" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="V147" s="2">
-        <v>15.393599999999999</v>
+        <v>14.5839</v>
       </c>
       <c r="W147" s="2">
-        <v>-87.7898</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23">
+        <v>-88.584599999999995</v>
+      </c>
+      <c r="AA147" s="8"/>
+    </row>
+    <row r="148" spans="1:27">
       <c r="A148" s="1">
         <v>28151</v>
       </c>
@@ -11672,40 +11679,40 @@
         <v>13</v>
       </c>
       <c r="F148" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G148" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G148" s="1" t="s">
+      <c r="H148" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" s="1">
+        <v>1</v>
+      </c>
+      <c r="J148" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H148" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I148" s="1">
-        <v>1</v>
-      </c>
-      <c r="J148" s="1" t="s">
+      <c r="K148" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K148" s="1" t="s">
+      <c r="L148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M148" s="1">
+        <v>1</v>
+      </c>
+      <c r="N148" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L148" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M148" s="1">
-        <v>1</v>
-      </c>
-      <c r="N148" s="1" t="s">
+      <c r="O148" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q148" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P148" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q148" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="R148" s="1" t="s">
         <v>34</v>
@@ -11717,13 +11724,13 @@
         <v>145</v>
       </c>
       <c r="V148" s="2">
-        <v>15.395200000000001</v>
+        <v>14.587899999999999</v>
       </c>
       <c r="W148" s="2">
-        <v>-87.808099999999996</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23">
+        <v>-88.582999999999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:27">
       <c r="A149" s="1">
         <v>28156</v>
       </c>
@@ -11740,58 +11747,58 @@
         <v>13</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G149" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="H149" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="1">
+        <v>1</v>
+      </c>
+      <c r="J149" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I149" s="1">
-        <v>1</v>
-      </c>
-      <c r="J149" s="1" t="s">
+      <c r="K149" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K149" s="1" t="s">
+      <c r="L149" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M149" s="1">
+        <v>1</v>
+      </c>
+      <c r="N149" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M149" s="1">
-        <v>1</v>
-      </c>
-      <c r="N149" s="1" t="s">
+      <c r="O149" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q149" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O149" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P149" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q149" s="1" t="s">
+      <c r="R149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U149" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="R149" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S149" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U149" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="V149" s="2">
-        <v>15.3955</v>
+        <v>14.588200000000001</v>
       </c>
       <c r="W149" s="2">
-        <v>-87.797700000000006</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23">
+        <v>-88.582700000000003</v>
+      </c>
+    </row>
+    <row r="150" spans="1:27">
       <c r="A150" s="1">
         <v>28181</v>
       </c>
@@ -11808,41 +11815,41 @@
         <v>13</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G150" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G150" s="1" t="s">
+      <c r="H150" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" s="1">
+        <v>1</v>
+      </c>
+      <c r="J150" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H150" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I150" s="1">
-        <v>1</v>
-      </c>
-      <c r="J150" s="1" t="s">
+      <c r="K150" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K150" s="1" t="s">
+      <c r="L150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M150" s="1">
+        <v>1</v>
+      </c>
+      <c r="N150" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L150" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M150" s="1">
-        <v>1</v>
-      </c>
-      <c r="N150" s="1" t="s">
+      <c r="O150" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q150" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O150" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P150" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="R150" s="1" t="s">
         <v>34</v>
       </c>
@@ -11850,16 +11857,16 @@
         <v>35</v>
       </c>
       <c r="U150" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V150" s="2">
-        <v>15.3956</v>
+        <v>14.588800000000001</v>
       </c>
       <c r="W150" s="2">
-        <v>-87.808400000000006</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23">
+        <v>-88.581699999999998</v>
+      </c>
+    </row>
+    <row r="151" spans="1:27">
       <c r="A151" s="1">
         <v>28327</v>
       </c>
@@ -11876,41 +11883,41 @@
         <v>13</v>
       </c>
       <c r="F151" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G151" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G151" s="1" t="s">
+      <c r="H151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="1">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H151" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I151" s="1">
-        <v>1</v>
-      </c>
-      <c r="J151" s="1" t="s">
+      <c r="K151" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K151" s="1" t="s">
+      <c r="L151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M151" s="1">
+        <v>1</v>
+      </c>
+      <c r="N151" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L151" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M151" s="1">
-        <v>1</v>
-      </c>
-      <c r="N151" s="1" t="s">
+      <c r="O151" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q151" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O151" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q151" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="R151" s="1" t="s">
         <v>34</v>
       </c>
@@ -11918,16 +11925,16 @@
         <v>35</v>
       </c>
       <c r="U151" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V151" s="2">
-        <v>15.3956</v>
+        <v>14.5922</v>
       </c>
       <c r="W151" s="2">
-        <v>-87.808499999999995</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23">
+        <v>-88.5822</v>
+      </c>
+    </row>
+    <row r="152" spans="1:27">
       <c r="A152" s="1">
         <v>33574</v>
       </c>
@@ -11944,10 +11951,10 @@
         <v>18</v>
       </c>
       <c r="F152" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>27</v>
@@ -11956,28 +11963,28 @@
         <v>4</v>
       </c>
       <c r="J152" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K152" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K152" s="1" t="s">
+      <c r="L152" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M152" s="1">
+        <v>1</v>
+      </c>
+      <c r="N152" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L152" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M152" s="1">
-        <v>1</v>
-      </c>
-      <c r="N152" s="1" t="s">
+      <c r="O152" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P152" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q152" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O152" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P152" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q152" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>34</v>
@@ -11989,13 +11996,13 @@
         <v>37</v>
       </c>
       <c r="V152" s="2">
-        <v>15.396100000000001</v>
+        <v>15.3992</v>
       </c>
       <c r="W152" s="2">
-        <v>-87.802400000000006</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23">
+        <v>-87.804299999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:27">
       <c r="A153" s="1">
         <v>33581</v>
       </c>
@@ -12012,10 +12019,10 @@
         <v>18</v>
       </c>
       <c r="F153" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>27</v>
@@ -12024,28 +12031,28 @@
         <v>4</v>
       </c>
       <c r="J153" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K153" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K153" s="1" t="s">
+      <c r="L153" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M153" s="1">
+        <v>1</v>
+      </c>
+      <c r="N153" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L153" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M153" s="1">
-        <v>1</v>
-      </c>
-      <c r="N153" s="1" t="s">
+      <c r="O153" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P153" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q153" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O153" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P153" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q153" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>34</v>
@@ -12057,13 +12064,13 @@
         <v>104</v>
       </c>
       <c r="V153" s="2">
-        <v>15.3971</v>
+        <v>15.400499999999999</v>
       </c>
       <c r="W153" s="2">
-        <v>-87.814599999999999</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23">
+        <v>-87.809700000000007</v>
+      </c>
+    </row>
+    <row r="154" spans="1:27">
       <c r="A154" s="1">
         <v>33592</v>
       </c>
@@ -12080,10 +12087,10 @@
         <v>18</v>
       </c>
       <c r="F154" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G154" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>27</v>
@@ -12092,28 +12099,28 @@
         <v>4</v>
       </c>
       <c r="J154" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K154" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K154" s="1" t="s">
+      <c r="L154" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M154" s="1">
+        <v>1</v>
+      </c>
+      <c r="N154" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L154" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M154" s="1">
-        <v>1</v>
-      </c>
-      <c r="N154" s="1" t="s">
+      <c r="O154" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P154" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q154" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O154" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P154" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q154" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>34</v>
@@ -12125,13 +12132,13 @@
         <v>106</v>
       </c>
       <c r="V154" s="2">
-        <v>15.3978</v>
+        <v>15.4011</v>
       </c>
       <c r="W154" s="2">
-        <v>-87.800399999999996</v>
-      </c>
-    </row>
-    <row r="155" spans="1:23">
+        <v>-87.809600000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:27">
       <c r="A155" s="1">
         <v>33598</v>
       </c>
@@ -12148,10 +12155,10 @@
         <v>18</v>
       </c>
       <c r="F155" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G155" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H155" s="1" t="s">
         <v>27</v>
@@ -12160,28 +12167,28 @@
         <v>4</v>
       </c>
       <c r="J155" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K155" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K155" s="1" t="s">
+      <c r="L155" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M155" s="1">
+        <v>1</v>
+      </c>
+      <c r="N155" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L155" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M155" s="1">
-        <v>1</v>
-      </c>
-      <c r="N155" s="1" t="s">
+      <c r="O155" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P155" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q155" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O155" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P155" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q155" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>34</v>
@@ -12193,13 +12200,13 @@
         <v>120</v>
       </c>
       <c r="V155" s="2">
-        <v>15.398099999999999</v>
+        <v>15.401400000000001</v>
       </c>
       <c r="W155" s="2">
-        <v>-87.814400000000006</v>
-      </c>
-    </row>
-    <row r="156" spans="1:23">
+        <v>-87.806600000000003</v>
+      </c>
+    </row>
+    <row r="156" spans="1:27">
       <c r="A156" s="1">
         <v>33636</v>
       </c>
@@ -12216,10 +12223,10 @@
         <v>18</v>
       </c>
       <c r="F156" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G156" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>27</v>
@@ -12228,28 +12235,28 @@
         <v>4</v>
       </c>
       <c r="J156" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K156" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K156" s="1" t="s">
+      <c r="L156" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M156" s="1">
+        <v>1</v>
+      </c>
+      <c r="N156" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L156" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M156" s="1">
-        <v>1</v>
-      </c>
-      <c r="N156" s="1" t="s">
+      <c r="O156" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P156" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q156" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O156" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P156" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q156" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>34</v>
@@ -12261,13 +12268,13 @@
         <v>104</v>
       </c>
       <c r="V156" s="2">
-        <v>15.398199999999999</v>
+        <v>15.402799999999999</v>
       </c>
       <c r="W156" s="2">
-        <v>-87.801699999999997</v>
-      </c>
-    </row>
-    <row r="157" spans="1:23">
+        <v>-87.806399999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:27">
       <c r="A157" s="1">
         <v>33637</v>
       </c>
@@ -12284,10 +12291,10 @@
         <v>18</v>
       </c>
       <c r="F157" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G157" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>27</v>
@@ -12296,28 +12303,28 @@
         <v>4</v>
       </c>
       <c r="J157" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K157" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K157" s="1" t="s">
+      <c r="L157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M157" s="1">
+        <v>1</v>
+      </c>
+      <c r="N157" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L157" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M157" s="1">
-        <v>1</v>
-      </c>
-      <c r="N157" s="1" t="s">
+      <c r="O157" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P157" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q157" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O157" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P157" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q157" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>34</v>
@@ -12329,13 +12336,13 @@
         <v>104</v>
       </c>
       <c r="V157" s="2">
-        <v>15.398300000000001</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W157" s="2">
-        <v>-87.809299999999993</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23">
+        <v>-87.806399999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:27">
       <c r="A158" s="1">
         <v>33638</v>
       </c>
@@ -12352,10 +12359,10 @@
         <v>18</v>
       </c>
       <c r="F158" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G158" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>27</v>
@@ -12364,28 +12371,28 @@
         <v>4</v>
       </c>
       <c r="J158" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K158" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K158" s="1" t="s">
+      <c r="L158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M158" s="1">
+        <v>1</v>
+      </c>
+      <c r="N158" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L158" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M158" s="1">
-        <v>1</v>
-      </c>
-      <c r="N158" s="1" t="s">
+      <c r="O158" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P158" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q158" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O158" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P158" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q158" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>34</v>
@@ -12397,13 +12404,13 @@
         <v>104</v>
       </c>
       <c r="V158" s="2">
-        <v>15.398300000000001</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W158" s="2">
-        <v>-87.809299999999993</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23">
+        <v>-87.806399999999996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:27">
       <c r="A159" s="1">
         <v>33647</v>
       </c>
@@ -12420,10 +12427,10 @@
         <v>18</v>
       </c>
       <c r="F159" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G159" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12432,46 +12439,46 @@
         <v>4</v>
       </c>
       <c r="J159" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K159" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K159" s="1" t="s">
+      <c r="L159" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M159" s="1">
+        <v>1</v>
+      </c>
+      <c r="N159" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L159" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M159" s="1">
-        <v>1</v>
-      </c>
-      <c r="N159" s="1" t="s">
+      <c r="O159" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P159" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q159" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="O159" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P159" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q159" s="1" t="s">
+      <c r="R159" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S159" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U159" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="R159" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S159" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U159" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="V159" s="2">
-        <v>15.399100000000001</v>
+        <v>15.403</v>
       </c>
       <c r="W159" s="2">
-        <v>-87.803799999999995</v>
-      </c>
-    </row>
-    <row r="160" spans="1:23">
+        <v>-87.805800000000005</v>
+      </c>
+    </row>
+    <row r="160" spans="1:27">
       <c r="A160" s="1">
         <v>33654</v>
       </c>
@@ -12488,10 +12495,10 @@
         <v>18</v>
       </c>
       <c r="F160" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
@@ -12500,29 +12507,29 @@
         <v>4</v>
       </c>
       <c r="J160" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K160" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K160" s="1" t="s">
+      <c r="L160" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M160" s="1">
+        <v>1</v>
+      </c>
+      <c r="N160" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L160" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M160" s="1">
-        <v>1</v>
-      </c>
-      <c r="N160" s="1" t="s">
+      <c r="O160" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P160" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q160" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="O160" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P160" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q160" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="R160" s="1" t="s">
         <v>34</v>
       </c>
@@ -12530,16 +12537,16 @@
         <v>35</v>
       </c>
       <c r="U160" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="V160" s="2">
-        <v>15.3992</v>
+        <v>15.4034</v>
       </c>
       <c r="W160" s="2">
-        <v>-87.804299999999998</v>
-      </c>
-    </row>
-    <row r="161" spans="1:23">
+        <v>-87.798599999999993</v>
+      </c>
+    </row>
+    <row r="161" spans="1:27">
       <c r="A161" s="1">
         <v>33662</v>
       </c>
@@ -12556,10 +12563,10 @@
         <v>18</v>
       </c>
       <c r="F161" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G161" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
@@ -12568,28 +12575,28 @@
         <v>4</v>
       </c>
       <c r="J161" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K161" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K161" s="1" t="s">
+      <c r="L161" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M161" s="1">
+        <v>1</v>
+      </c>
+      <c r="N161" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L161" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M161" s="1">
-        <v>1</v>
-      </c>
-      <c r="N161" s="1" t="s">
+      <c r="O161" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P161" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q161" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O161" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P161" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q161" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>34</v>
@@ -12601,13 +12608,13 @@
         <v>37</v>
       </c>
       <c r="V161" s="2">
-        <v>15.3995</v>
+        <v>15.404199999999999</v>
       </c>
       <c r="W161" s="2">
-        <v>-87.8078</v>
-      </c>
-    </row>
-    <row r="162" spans="1:23">
+        <v>-87.812100000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:27" ht="15">
       <c r="A162" s="1">
         <v>33664</v>
       </c>
@@ -12624,10 +12631,10 @@
         <v>18</v>
       </c>
       <c r="F162" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G162" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
@@ -12636,28 +12643,28 @@
         <v>4</v>
       </c>
       <c r="J162" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K162" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K162" s="1" t="s">
+      <c r="L162" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M162" s="1">
+        <v>1</v>
+      </c>
+      <c r="N162" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L162" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M162" s="1">
-        <v>1</v>
-      </c>
-      <c r="N162" s="1" t="s">
+      <c r="O162" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P162" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q162" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O162" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P162" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q162" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>34</v>
@@ -12669,11 +12676,12 @@
         <v>62</v>
       </c>
       <c r="V162" s="2">
-        <v>15.399699999999999</v>
+        <v>15.404500000000001</v>
       </c>
       <c r="W162" s="2">
-        <v>-87.811000000000007</v>
-      </c>
+        <v>-87.808999999999997</v>
+      </c>
+      <c r="AA162" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U162">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-22-2020 04-29-00
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2959EC4F-AEF0-4A40-8DB9-92839F6B497D}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{133B870B-09C0-4216-8C99-C73D3287A0DA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="FARMACIAS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$162</definedName>
-    <definedName name="_xlnm.Database">FARMACIAS!$A$1:$U$162</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$179</definedName>
+    <definedName name="_xlnm.Database">FARMACIAS!$A$1:$U$160</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="221">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -279,15 +279,15 @@
     <t>Comayagua</t>
   </si>
   <si>
+    <t>030101</t>
+  </si>
+  <si>
+    <t>HND-0301</t>
+  </si>
+  <si>
     <t>0301</t>
   </si>
   <si>
-    <t>030101</t>
-  </si>
-  <si>
-    <t>HND-0301</t>
-  </si>
-  <si>
     <t>Farmacia Colonial</t>
   </si>
   <si>
@@ -643,6 +643,60 @@
   </si>
   <si>
     <t>HND-1102</t>
+  </si>
+  <si>
+    <t>aldea</t>
+  </si>
+  <si>
+    <t>Farmacias kielsa Siguatepeque</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Siguatepeque #1</t>
+  </si>
+  <si>
+    <t>Farmacia Montecristo</t>
+  </si>
+  <si>
+    <t>Farmacia Kielsa</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Siguatepeque #3</t>
+  </si>
+  <si>
+    <t>Farmacia el Angel</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Siguatepeque #4</t>
+  </si>
+  <si>
+    <t>Farmacia Recinos</t>
+  </si>
+  <si>
+    <t>Farmacia Nuevo Sol</t>
+  </si>
+  <si>
+    <t>Tochis Farmacia</t>
+  </si>
+  <si>
+    <t>Pronavida</t>
+  </si>
+  <si>
+    <t>Farmacia Milla</t>
+  </si>
+  <si>
+    <t>farmacia city</t>
+  </si>
+  <si>
+    <t>Kielsa</t>
+  </si>
+  <si>
+    <t>Farmacia Nahualí</t>
+  </si>
+  <si>
+    <t>Medi7</t>
+  </si>
+  <si>
+    <t>FarmaCity Calle 21 de agosto</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1197,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1153,6 +1207,8 @@
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1301,10 +1357,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W162" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W162" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W162">
-    <sortCondition ref="A1:A162"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W179" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W179" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W160">
+    <sortCondition ref="A1:A160"/>
   </sortState>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{C232FE6F-7903-4FC5-93EC-F7BD24958957}" name="OBJECTID_1" dataDxfId="22"/>
@@ -1632,11 +1688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA162"/>
+  <dimension ref="A1:AA185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z26" sqref="Z26"/>
+      <pane ySplit="1" topLeftCell="P167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -6252,8 +6308,8 @@
       <c r="I68" s="1">
         <v>1</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>81</v>
+      <c r="J68" s="1">
+        <v>301</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>80</v>
@@ -6265,7 +6321,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O68" s="1" t="s">
         <v>80</v>
@@ -6274,7 +6330,7 @@
         <v>33</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R68" s="1" t="s">
         <v>35</v>
@@ -6321,7 +6377,7 @@
         <v>1</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>80</v>
@@ -6333,7 +6389,7 @@
         <v>1</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O69" s="1" t="s">
         <v>80</v>
@@ -6342,7 +6398,7 @@
         <v>33</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R69" s="1" t="s">
         <v>35</v>
@@ -6389,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>80</v>
@@ -6401,7 +6457,7 @@
         <v>1</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>80</v>
@@ -6410,7 +6466,7 @@
         <v>33</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R70" s="1" t="s">
         <v>35</v>
@@ -6457,7 +6513,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>80</v>
@@ -6469,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>80</v>
@@ -6478,7 +6534,7 @@
         <v>33</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R71" s="1" t="s">
         <v>35</v>
@@ -6525,7 +6581,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>80</v>
@@ -6537,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O72" s="1" t="s">
         <v>80</v>
@@ -6546,7 +6602,7 @@
         <v>33</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R72" s="1" t="s">
         <v>35</v>
@@ -6593,7 +6649,7 @@
         <v>1</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>80</v>
@@ -6605,7 +6661,7 @@
         <v>1</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O73" s="1" t="s">
         <v>80</v>
@@ -6614,7 +6670,7 @@
         <v>33</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R73" s="1" t="s">
         <v>35</v>
@@ -7518,7 +7574,7 @@
     </row>
     <row r="87" spans="1:23">
       <c r="A87" s="1">
-        <v>28499</v>
+        <v>28512</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>23</v>
@@ -7575,86 +7631,87 @@
         <v>36</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="V87" s="2">
-        <v>14.596399999999999</v>
+        <v>14.596500000000001</v>
       </c>
       <c r="W87" s="2">
-        <v>-87.831199999999995</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23">
-      <c r="A88" s="1">
-        <v>28512</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D88" s="1">
-        <v>3</v>
-      </c>
-      <c r="E88" s="1">
-        <v>3</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="1">
-        <v>18</v>
-      </c>
-      <c r="J88" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L88" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M88" s="1">
-        <v>1</v>
-      </c>
-      <c r="N88" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O88" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="P88" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q88" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="R88" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S88" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U88" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="V88" s="2">
-        <v>14.596500000000001</v>
-      </c>
-      <c r="W88" s="2">
         <v>-87.832300000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" s="8" customFormat="1" ht="15">
+      <c r="A88" s="9">
+        <v>31814</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="9">
+        <v>3</v>
+      </c>
+      <c r="E88" s="9">
+        <v>4</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="9">
+        <v>1</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K88" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L88" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M88" s="9">
+        <v>1</v>
+      </c>
+      <c r="N88" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="O88" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="P88" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q88" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="R88" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S88" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T88" s="9"/>
+      <c r="U88" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V88" s="10">
+        <v>14.767799999999999</v>
+      </c>
+      <c r="W88" s="10">
+        <v>-88.779300000000006</v>
       </c>
     </row>
     <row r="89" spans="1:23">
       <c r="A89" s="1">
-        <v>28641</v>
+        <v>31817</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>23</v>
@@ -7666,25 +7723,25 @@
         <v>3</v>
       </c>
       <c r="E89" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I89" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>30</v>
@@ -7693,16 +7750,16 @@
         <v>1</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="P89" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="R89" s="1" t="s">
         <v>35</v>
@@ -7711,18 +7768,18 @@
         <v>36</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="V89" s="2">
-        <v>14.598699999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W89" s="2">
-        <v>-87.831400000000002</v>
+        <v>-88.777600000000007</v>
       </c>
     </row>
     <row r="90" spans="1:23">
       <c r="A90" s="1">
-        <v>31814</v>
+        <v>31819</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>23</v>
@@ -7779,18 +7836,18 @@
         <v>36</v>
       </c>
       <c r="U90" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V90" s="2">
-        <v>14.767799999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W90" s="2">
-        <v>-88.779300000000006</v>
+        <v>-88.777500000000003</v>
       </c>
     </row>
     <row r="91" spans="1:23">
       <c r="A91" s="1">
-        <v>31817</v>
+        <v>32195</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>23</v>
@@ -7814,13 +7871,13 @@
         <v>27</v>
       </c>
       <c r="I91" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>30</v>
@@ -7829,16 +7886,16 @@
         <v>1</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="P91" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="R91" s="1" t="s">
         <v>35</v>
@@ -7847,18 +7904,18 @@
         <v>36</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="V91" s="2">
-        <v>14.7681</v>
+        <v>14.832100000000001</v>
       </c>
       <c r="W91" s="2">
-        <v>-88.777600000000007</v>
+        <v>-89.093999999999994</v>
       </c>
     </row>
     <row r="92" spans="1:23">
       <c r="A92" s="1">
-        <v>31819</v>
+        <v>32419</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>23</v>
@@ -7882,13 +7939,13 @@
         <v>27</v>
       </c>
       <c r="I92" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>30</v>
@@ -7897,16 +7954,16 @@
         <v>1</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="P92" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="R92" s="1" t="s">
         <v>35</v>
@@ -7915,18 +7972,18 @@
         <v>36</v>
       </c>
       <c r="U92" s="1" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="V92" s="2">
-        <v>14.7681</v>
+        <v>14.8384</v>
       </c>
       <c r="W92" s="2">
-        <v>-88.777500000000003</v>
+        <v>-89.1554</v>
       </c>
     </row>
     <row r="93" spans="1:23">
       <c r="A93" s="1">
-        <v>32195</v>
+        <v>33156</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>23</v>
@@ -7950,13 +8007,13 @@
         <v>27</v>
       </c>
       <c r="I93" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>30</v>
@@ -7965,16 +8022,16 @@
         <v>1</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="P93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="R93" s="1" t="s">
         <v>35</v>
@@ -7983,18 +8040,18 @@
         <v>36</v>
       </c>
       <c r="U93" s="1" t="s">
-        <v>123</v>
+        <v>48</v>
       </c>
       <c r="V93" s="2">
-        <v>14.832100000000001</v>
+        <v>15.065799999999999</v>
       </c>
       <c r="W93" s="2">
-        <v>-89.093999999999994</v>
+        <v>-88.747100000000003</v>
       </c>
     </row>
     <row r="94" spans="1:23">
       <c r="A94" s="1">
-        <v>32419</v>
+        <v>33366</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>23</v>
@@ -8006,25 +8063,25 @@
         <v>3</v>
       </c>
       <c r="E94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I94" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>30</v>
@@ -8033,16 +8090,16 @@
         <v>1</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="P94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="R94" s="1" t="s">
         <v>35</v>
@@ -8051,18 +8108,18 @@
         <v>36</v>
       </c>
       <c r="U94" s="1" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="V94" s="2">
-        <v>14.8384</v>
+        <v>15.316800000000001</v>
       </c>
       <c r="W94" s="2">
-        <v>-89.1554</v>
+        <v>-87.990300000000005</v>
       </c>
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="1">
-        <v>33156</v>
+        <v>33574</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>23</v>
@@ -8074,25 +8131,25 @@
         <v>3</v>
       </c>
       <c r="E95" s="1">
+        <v>18</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I95" s="1">
         <v>4</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I95" s="1">
-        <v>13</v>
-      </c>
       <c r="J95" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>30</v>
@@ -8101,16 +8158,16 @@
         <v>1</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="P95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="R95" s="1" t="s">
         <v>35</v>
@@ -8119,18 +8176,18 @@
         <v>36</v>
       </c>
       <c r="U95" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V95" s="2">
-        <v>15.065799999999999</v>
+        <v>15.3992</v>
       </c>
       <c r="W95" s="2">
-        <v>-88.747100000000003</v>
+        <v>-87.804299999999998</v>
       </c>
     </row>
     <row r="96" spans="1:23">
       <c r="A96" s="1">
-        <v>33366</v>
+        <v>33581</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>23</v>
@@ -8142,25 +8199,25 @@
         <v>3</v>
       </c>
       <c r="E96" s="1">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I96" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>30</v>
@@ -8169,16 +8226,16 @@
         <v>1</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="P96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q96" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="R96" s="1" t="s">
         <v>35</v>
@@ -8187,18 +8244,18 @@
         <v>36</v>
       </c>
       <c r="U96" s="1" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="V96" s="2">
-        <v>15.316800000000001</v>
+        <v>15.400499999999999</v>
       </c>
       <c r="W96" s="2">
-        <v>-87.990300000000005</v>
+        <v>-87.809700000000007</v>
       </c>
     </row>
     <row r="97" spans="1:23">
       <c r="A97" s="1">
-        <v>33574</v>
+        <v>33592</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>23</v>
@@ -8255,18 +8312,18 @@
         <v>36</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="V97" s="2">
-        <v>15.3992</v>
+        <v>15.4011</v>
       </c>
       <c r="W97" s="2">
-        <v>-87.804299999999998</v>
+        <v>-87.809600000000003</v>
       </c>
     </row>
     <row r="98" spans="1:23">
       <c r="A98" s="1">
-        <v>33581</v>
+        <v>33598</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>23</v>
@@ -8323,18 +8380,18 @@
         <v>36</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V98" s="2">
-        <v>15.400499999999999</v>
+        <v>15.401400000000001</v>
       </c>
       <c r="W98" s="2">
-        <v>-87.809700000000007</v>
+        <v>-87.806600000000003</v>
       </c>
     </row>
     <row r="99" spans="1:23">
       <c r="A99" s="1">
-        <v>33592</v>
+        <v>33636</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>23</v>
@@ -8391,18 +8448,18 @@
         <v>36</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="V99" s="2">
-        <v>15.4011</v>
+        <v>15.402799999999999</v>
       </c>
       <c r="W99" s="2">
-        <v>-87.809600000000003</v>
+        <v>-87.806399999999996</v>
       </c>
     </row>
     <row r="100" spans="1:23">
       <c r="A100" s="1">
-        <v>33598</v>
+        <v>33637</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>23</v>
@@ -8459,18 +8516,18 @@
         <v>36</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="V100" s="2">
-        <v>15.401400000000001</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W100" s="2">
-        <v>-87.806600000000003</v>
+        <v>-87.806399999999996</v>
       </c>
     </row>
     <row r="101" spans="1:23">
       <c r="A101" s="1">
-        <v>33636</v>
+        <v>33638</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>23</v>
@@ -8530,7 +8587,7 @@
         <v>146</v>
       </c>
       <c r="V101" s="2">
-        <v>15.402799999999999</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W101" s="2">
         <v>-87.806399999999996</v>
@@ -8538,7 +8595,7 @@
     </row>
     <row r="102" spans="1:23">
       <c r="A102" s="1">
-        <v>33637</v>
+        <v>33647</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>23</v>
@@ -8595,18 +8652,18 @@
         <v>36</v>
       </c>
       <c r="U102" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="V102" s="2">
-        <v>15.402900000000001</v>
+        <v>15.403</v>
       </c>
       <c r="W102" s="2">
-        <v>-87.806399999999996</v>
+        <v>-87.805800000000005</v>
       </c>
     </row>
     <row r="103" spans="1:23">
       <c r="A103" s="1">
-        <v>33638</v>
+        <v>33654</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>23</v>
@@ -8663,18 +8720,18 @@
         <v>36</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="V103" s="2">
-        <v>15.402900000000001</v>
+        <v>15.4034</v>
       </c>
       <c r="W103" s="2">
-        <v>-87.806399999999996</v>
+        <v>-87.798599999999993</v>
       </c>
     </row>
     <row r="104" spans="1:23">
       <c r="A104" s="1">
-        <v>33647</v>
+        <v>33662</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>23</v>
@@ -8731,18 +8788,18 @@
         <v>36</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="V104" s="2">
-        <v>15.403</v>
+        <v>15.404199999999999</v>
       </c>
       <c r="W104" s="2">
-        <v>-87.805800000000005</v>
+        <v>-87.812100000000001</v>
       </c>
     </row>
     <row r="105" spans="1:23">
       <c r="A105" s="1">
-        <v>33654</v>
+        <v>33664</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>23</v>
@@ -8799,18 +8856,18 @@
         <v>36</v>
       </c>
       <c r="U105" s="1" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="V105" s="2">
-        <v>15.4034</v>
+        <v>15.404500000000001</v>
       </c>
       <c r="W105" s="2">
-        <v>-87.798599999999993</v>
+        <v>-87.808999999999997</v>
       </c>
     </row>
     <row r="106" spans="1:23">
       <c r="A106" s="1">
-        <v>33662</v>
+        <v>33766</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>23</v>
@@ -8822,25 +8879,25 @@
         <v>3</v>
       </c>
       <c r="E106" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I106" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L106" s="1" t="s">
         <v>30</v>
@@ -8849,16 +8906,16 @@
         <v>1</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="P106" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="R106" s="1" t="s">
         <v>35</v>
@@ -8870,15 +8927,15 @@
         <v>41</v>
       </c>
       <c r="V106" s="2">
-        <v>15.404199999999999</v>
+        <v>15.4361</v>
       </c>
       <c r="W106" s="2">
-        <v>-87.812100000000001</v>
+        <v>-87.921099999999996</v>
       </c>
     </row>
     <row r="107" spans="1:23">
       <c r="A107" s="1">
-        <v>33664</v>
+        <v>33767</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>23</v>
@@ -8890,25 +8947,25 @@
         <v>3</v>
       </c>
       <c r="E107" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I107" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>30</v>
@@ -8917,16 +8974,16 @@
         <v>1</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="P107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="R107" s="1" t="s">
         <v>35</v>
@@ -8938,15 +8995,15 @@
         <v>56</v>
       </c>
       <c r="V107" s="2">
-        <v>15.404500000000001</v>
+        <v>15.436500000000001</v>
       </c>
       <c r="W107" s="2">
-        <v>-87.808999999999997</v>
+        <v>-87.924300000000002</v>
       </c>
     </row>
     <row r="108" spans="1:23">
       <c r="A108" s="1">
-        <v>33766</v>
+        <v>33773</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>23</v>
@@ -9006,15 +9063,15 @@
         <v>41</v>
       </c>
       <c r="V108" s="2">
-        <v>15.4361</v>
+        <v>15.438499999999999</v>
       </c>
       <c r="W108" s="2">
-        <v>-87.921099999999996</v>
+        <v>-87.926900000000003</v>
       </c>
     </row>
     <row r="109" spans="1:23">
       <c r="A109" s="1">
-        <v>33767</v>
+        <v>33778</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>23</v>
@@ -9071,18 +9128,18 @@
         <v>36</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="V109" s="2">
-        <v>15.436500000000001</v>
+        <v>15.4405</v>
       </c>
       <c r="W109" s="2">
-        <v>-87.924300000000002</v>
+        <v>-87.929100000000005</v>
       </c>
     </row>
     <row r="110" spans="1:23">
       <c r="A110" s="1">
-        <v>33773</v>
+        <v>33918</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>23</v>
@@ -9106,13 +9163,13 @@
         <v>27</v>
       </c>
       <c r="I110" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>30</v>
@@ -9121,16 +9178,16 @@
         <v>1</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="O110" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="P110" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="R110" s="1" t="s">
         <v>35</v>
@@ -9142,15 +9199,15 @@
         <v>41</v>
       </c>
       <c r="V110" s="2">
-        <v>15.438499999999999</v>
+        <v>15.477399999999999</v>
       </c>
       <c r="W110" s="2">
-        <v>-87.926900000000003</v>
+        <v>-87.985699999999994</v>
       </c>
     </row>
     <row r="111" spans="1:23">
       <c r="A111" s="1">
-        <v>33778</v>
+        <v>33929</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>23</v>
@@ -9174,13 +9231,13 @@
         <v>27</v>
       </c>
       <c r="I111" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>30</v>
@@ -9189,16 +9246,16 @@
         <v>1</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="O111" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="P111" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="R111" s="1" t="s">
         <v>35</v>
@@ -9207,18 +9264,18 @@
         <v>36</v>
       </c>
       <c r="U111" s="1" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="V111" s="2">
-        <v>15.4405</v>
+        <v>15.4787</v>
       </c>
       <c r="W111" s="2">
-        <v>-87.929100000000005</v>
+        <v>-87.975099999999998</v>
       </c>
     </row>
     <row r="112" spans="1:23">
       <c r="A112" s="1">
-        <v>33918</v>
+        <v>33941</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>23</v>
@@ -9275,18 +9332,18 @@
         <v>36</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
       <c r="V112" s="2">
-        <v>15.477399999999999</v>
+        <v>15.4796</v>
       </c>
       <c r="W112" s="2">
-        <v>-87.985699999999994</v>
+        <v>-88.011200000000002</v>
       </c>
     </row>
     <row r="113" spans="1:23">
       <c r="A113" s="1">
-        <v>33929</v>
+        <v>33960</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>23</v>
@@ -9343,18 +9400,18 @@
         <v>36</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="V113" s="2">
-        <v>15.4787</v>
+        <v>15.4854</v>
       </c>
       <c r="W113" s="2">
-        <v>-87.975099999999998</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="114" spans="1:23">
       <c r="A114" s="1">
-        <v>33941</v>
+        <v>33962</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>23</v>
@@ -9411,18 +9468,18 @@
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="V114" s="2">
-        <v>15.4796</v>
+        <v>15.4855</v>
       </c>
       <c r="W114" s="2">
-        <v>-88.011200000000002</v>
+        <v>-87.984399999999994</v>
       </c>
     </row>
     <row r="115" spans="1:23">
       <c r="A115" s="1">
-        <v>33960</v>
+        <v>33987</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>23</v>
@@ -9479,18 +9536,18 @@
         <v>36</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="V115" s="2">
-        <v>15.4854</v>
+        <v>15.489800000000001</v>
       </c>
       <c r="W115" s="2">
-        <v>-88.034099999999995</v>
+        <v>-87.986000000000004</v>
       </c>
     </row>
     <row r="116" spans="1:23">
       <c r="A116" s="1">
-        <v>33962</v>
+        <v>34003</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>23</v>
@@ -9547,18 +9604,18 @@
         <v>36</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="V116" s="2">
-        <v>15.4855</v>
+        <v>15.492599999999999</v>
       </c>
       <c r="W116" s="2">
-        <v>-87.984399999999994</v>
+        <v>-88.011499999999998</v>
       </c>
     </row>
     <row r="117" spans="1:23">
       <c r="A117" s="1">
-        <v>33987</v>
+        <v>34007</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>23</v>
@@ -9615,18 +9672,18 @@
         <v>36</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="V117" s="2">
-        <v>15.489800000000001</v>
+        <v>15.492699999999999</v>
       </c>
       <c r="W117" s="2">
-        <v>-87.986000000000004</v>
+        <v>-88.016499999999994</v>
       </c>
     </row>
     <row r="118" spans="1:23">
       <c r="A118" s="1">
-        <v>34003</v>
+        <v>34010</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>23</v>
@@ -9683,18 +9740,18 @@
         <v>36</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="V118" s="2">
-        <v>15.492599999999999</v>
+        <v>15.4933</v>
       </c>
       <c r="W118" s="2">
-        <v>-88.011499999999998</v>
+        <v>-87.986500000000007</v>
       </c>
     </row>
     <row r="119" spans="1:23">
       <c r="A119" s="1">
-        <v>34007</v>
+        <v>34011</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>23</v>
@@ -9754,15 +9811,15 @@
         <v>41</v>
       </c>
       <c r="V119" s="2">
-        <v>15.492699999999999</v>
+        <v>15.493399999999999</v>
       </c>
       <c r="W119" s="2">
-        <v>-88.016499999999994</v>
+        <v>-87.984800000000007</v>
       </c>
     </row>
     <row r="120" spans="1:23">
       <c r="A120" s="1">
-        <v>34010</v>
+        <v>34016</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>23</v>
@@ -9822,15 +9879,15 @@
         <v>41</v>
       </c>
       <c r="V120" s="2">
-        <v>15.4933</v>
+        <v>15.493600000000001</v>
       </c>
       <c r="W120" s="2">
-        <v>-87.986500000000007</v>
+        <v>-87.984099999999998</v>
       </c>
     </row>
     <row r="121" spans="1:23">
       <c r="A121" s="1">
-        <v>34011</v>
+        <v>34030</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>23</v>
@@ -9887,18 +9944,18 @@
         <v>36</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="V121" s="2">
-        <v>15.493399999999999</v>
+        <v>15.494300000000001</v>
       </c>
       <c r="W121" s="2">
-        <v>-87.984800000000007</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="122" spans="1:23">
       <c r="A122" s="1">
-        <v>34016</v>
+        <v>34134</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>23</v>
@@ -9955,18 +10012,18 @@
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="V122" s="2">
-        <v>15.493600000000001</v>
+        <v>15.499700000000001</v>
       </c>
       <c r="W122" s="2">
-        <v>-87.984099999999998</v>
+        <v>-88.025000000000006</v>
       </c>
     </row>
     <row r="123" spans="1:23">
       <c r="A123" s="1">
-        <v>34030</v>
+        <v>34144</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>23</v>
@@ -10023,18 +10080,18 @@
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="V123" s="2">
-        <v>15.494300000000001</v>
+        <v>15.4999</v>
       </c>
       <c r="W123" s="2">
-        <v>-88.034099999999995</v>
+        <v>-88.037499999999994</v>
       </c>
     </row>
     <row r="124" spans="1:23">
       <c r="A124" s="1">
-        <v>34134</v>
+        <v>34146</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>23</v>
@@ -10091,18 +10148,18 @@
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="V124" s="2">
-        <v>15.499700000000001</v>
+        <v>15.5</v>
       </c>
       <c r="W124" s="2">
-        <v>-88.025000000000006</v>
+        <v>-88.020700000000005</v>
       </c>
     </row>
     <row r="125" spans="1:23">
       <c r="A125" s="1">
-        <v>34144</v>
+        <v>34160</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>23</v>
@@ -10159,18 +10216,18 @@
         <v>36</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="V125" s="2">
-        <v>15.4999</v>
+        <v>15.500299999999999</v>
       </c>
       <c r="W125" s="2">
-        <v>-88.037499999999994</v>
+        <v>-88.038399999999996</v>
       </c>
     </row>
     <row r="126" spans="1:23">
       <c r="A126" s="1">
-        <v>34146</v>
+        <v>34204</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>23</v>
@@ -10227,18 +10284,18 @@
         <v>36</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="V126" s="2">
-        <v>15.5</v>
+        <v>15.501799999999999</v>
       </c>
       <c r="W126" s="2">
-        <v>-88.020700000000005</v>
+        <v>-88.027100000000004</v>
       </c>
     </row>
     <row r="127" spans="1:23">
       <c r="A127" s="1">
-        <v>34160</v>
+        <v>34249</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>23</v>
@@ -10295,18 +10352,18 @@
         <v>36</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="V127" s="2">
-        <v>15.500299999999999</v>
+        <v>15.504099999999999</v>
       </c>
       <c r="W127" s="2">
-        <v>-88.038399999999996</v>
+        <v>-88.014200000000002</v>
       </c>
     </row>
     <row r="128" spans="1:23">
       <c r="A128" s="1">
-        <v>34204</v>
+        <v>34269</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>23</v>
@@ -10363,18 +10420,18 @@
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="V128" s="2">
-        <v>15.501799999999999</v>
+        <v>15.505100000000001</v>
       </c>
       <c r="W128" s="2">
-        <v>-88.027100000000004</v>
+        <v>-88.022300000000001</v>
       </c>
     </row>
     <row r="129" spans="1:23">
       <c r="A129" s="1">
-        <v>34249</v>
+        <v>34306</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>23</v>
@@ -10431,18 +10488,18 @@
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="V129" s="2">
-        <v>15.504099999999999</v>
+        <v>15.5061</v>
       </c>
       <c r="W129" s="2">
-        <v>-88.014200000000002</v>
+        <v>-88.027199999999993</v>
       </c>
     </row>
     <row r="130" spans="1:23">
       <c r="A130" s="1">
-        <v>34269</v>
+        <v>34359</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>23</v>
@@ -10499,18 +10556,18 @@
         <v>36</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>165</v>
+        <v>84</v>
       </c>
       <c r="V130" s="2">
-        <v>15.505100000000001</v>
+        <v>15.5105</v>
       </c>
       <c r="W130" s="2">
-        <v>-88.022300000000001</v>
+        <v>-88.012699999999995</v>
       </c>
     </row>
     <row r="131" spans="1:23">
       <c r="A131" s="1">
-        <v>34306</v>
+        <v>34373</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>23</v>
@@ -10567,18 +10624,18 @@
         <v>36</v>
       </c>
       <c r="U131" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="V131" s="2">
-        <v>15.5061</v>
+        <v>15.5124</v>
       </c>
       <c r="W131" s="2">
-        <v>-88.027199999999993</v>
+        <v>-88.037000000000006</v>
       </c>
     </row>
     <row r="132" spans="1:23">
       <c r="A132" s="1">
-        <v>34359</v>
+        <v>34389</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>23</v>
@@ -10635,18 +10692,18 @@
         <v>36</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="V132" s="2">
-        <v>15.5105</v>
+        <v>15.5146</v>
       </c>
       <c r="W132" s="2">
-        <v>-88.012699999999995</v>
+        <v>-88.033600000000007</v>
       </c>
     </row>
     <row r="133" spans="1:23">
       <c r="A133" s="1">
-        <v>34373</v>
+        <v>34401</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>23</v>
@@ -10706,15 +10763,15 @@
         <v>41</v>
       </c>
       <c r="V133" s="2">
-        <v>15.5124</v>
+        <v>15.5159</v>
       </c>
       <c r="W133" s="2">
-        <v>-88.037000000000006</v>
+        <v>-88.028400000000005</v>
       </c>
     </row>
     <row r="134" spans="1:23">
       <c r="A134" s="1">
-        <v>34389</v>
+        <v>34445</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>23</v>
@@ -10771,18 +10828,18 @@
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="V134" s="2">
-        <v>15.5146</v>
+        <v>15.5244</v>
       </c>
       <c r="W134" s="2">
-        <v>-88.033600000000007</v>
+        <v>-88.038499999999999</v>
       </c>
     </row>
     <row r="135" spans="1:23">
       <c r="A135" s="1">
-        <v>34401</v>
+        <v>34466</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>23</v>
@@ -10839,18 +10896,18 @@
         <v>36</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="V135" s="2">
-        <v>15.5159</v>
+        <v>15.5298</v>
       </c>
       <c r="W135" s="2">
-        <v>-88.028400000000005</v>
+        <v>-88.032700000000006</v>
       </c>
     </row>
     <row r="136" spans="1:23">
       <c r="A136" s="1">
-        <v>34445</v>
+        <v>34471</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>23</v>
@@ -10907,18 +10964,18 @@
         <v>36</v>
       </c>
       <c r="U136" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V136" s="2">
-        <v>15.5244</v>
+        <v>15.5299</v>
       </c>
       <c r="W136" s="2">
-        <v>-88.038499999999999</v>
+        <v>-88.026499999999999</v>
       </c>
     </row>
     <row r="137" spans="1:23">
       <c r="A137" s="1">
-        <v>34466</v>
+        <v>34475</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>23</v>
@@ -10975,18 +11032,18 @@
         <v>36</v>
       </c>
       <c r="U137" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="V137" s="2">
-        <v>15.5298</v>
+        <v>15.5299</v>
       </c>
       <c r="W137" s="2">
-        <v>-88.032700000000006</v>
+        <v>-88.025499999999994</v>
       </c>
     </row>
     <row r="138" spans="1:23">
       <c r="A138" s="1">
-        <v>34471</v>
+        <v>34521</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>23</v>
@@ -11043,18 +11100,18 @@
         <v>36</v>
       </c>
       <c r="U138" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="V138" s="2">
-        <v>15.5299</v>
+        <v>15.5306</v>
       </c>
       <c r="W138" s="2">
-        <v>-88.026499999999999</v>
+        <v>-88.029399999999995</v>
       </c>
     </row>
     <row r="139" spans="1:23">
       <c r="A139" s="1">
-        <v>34475</v>
+        <v>34533</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>23</v>
@@ -11111,18 +11168,18 @@
         <v>36</v>
       </c>
       <c r="U139" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V139" s="2">
-        <v>15.5299</v>
+        <v>15.5341</v>
       </c>
       <c r="W139" s="2">
-        <v>-88.025499999999994</v>
+        <v>-88.019300000000001</v>
       </c>
     </row>
     <row r="140" spans="1:23">
       <c r="A140" s="1">
-        <v>34521</v>
+        <v>34539</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>23</v>
@@ -11182,15 +11239,15 @@
         <v>48</v>
       </c>
       <c r="V140" s="2">
-        <v>15.5306</v>
+        <v>15.537100000000001</v>
       </c>
       <c r="W140" s="2">
-        <v>-88.029399999999995</v>
+        <v>-88.014899999999997</v>
       </c>
     </row>
     <row r="141" spans="1:23">
       <c r="A141" s="1">
-        <v>34533</v>
+        <v>34554</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>23</v>
@@ -11250,15 +11307,15 @@
         <v>41</v>
       </c>
       <c r="V141" s="2">
-        <v>15.5341</v>
+        <v>15.542899999999999</v>
       </c>
       <c r="W141" s="2">
-        <v>-88.019300000000001</v>
+        <v>-88.023099999999999</v>
       </c>
     </row>
     <row r="142" spans="1:23">
       <c r="A142" s="1">
-        <v>34539</v>
+        <v>34576</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>23</v>
@@ -11315,18 +11372,18 @@
         <v>36</v>
       </c>
       <c r="U142" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V142" s="2">
-        <v>15.537100000000001</v>
+        <v>15.549099999999999</v>
       </c>
       <c r="W142" s="2">
-        <v>-88.014899999999997</v>
+        <v>-88.035899999999998</v>
       </c>
     </row>
     <row r="143" spans="1:23">
       <c r="A143" s="1">
-        <v>34554</v>
+        <v>34583</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>23</v>
@@ -11386,15 +11443,15 @@
         <v>41</v>
       </c>
       <c r="V143" s="2">
-        <v>15.542899999999999</v>
+        <v>15.5505</v>
       </c>
       <c r="W143" s="2">
-        <v>-88.023099999999999</v>
+        <v>-88.004800000000003</v>
       </c>
     </row>
     <row r="144" spans="1:23">
       <c r="A144" s="1">
-        <v>34576</v>
+        <v>34671</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>23</v>
@@ -11406,43 +11463,43 @@
         <v>3</v>
       </c>
       <c r="E144" s="1">
+        <v>1</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="1">
         <v>5</v>
       </c>
-      <c r="F144" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I144" s="1">
-        <v>1</v>
-      </c>
       <c r="J144" s="1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="L144" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M144" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="O144" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P144" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q144" s="1" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="R144" s="1" t="s">
         <v>35</v>
@@ -11451,18 +11508,18 @@
         <v>36</v>
       </c>
       <c r="U144" s="1" t="s">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="V144" s="2">
-        <v>15.549099999999999</v>
+        <v>15.5989</v>
       </c>
       <c r="W144" s="2">
-        <v>-88.035899999999998</v>
-      </c>
-    </row>
-    <row r="145" spans="1:27">
+        <v>-87.208799999999997</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27" ht="15">
       <c r="A145" s="1">
-        <v>34583</v>
+        <v>34675</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>23</v>
@@ -11474,43 +11531,43 @@
         <v>3</v>
       </c>
       <c r="E145" s="1">
+        <v>1</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I145" s="1">
         <v>5</v>
       </c>
-      <c r="F145" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H145" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I145" s="1">
-        <v>1</v>
-      </c>
       <c r="J145" s="1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M145" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P145" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="R145" s="1" t="s">
         <v>35</v>
@@ -11519,18 +11576,19 @@
         <v>36</v>
       </c>
       <c r="U145" s="1" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="V145" s="2">
-        <v>15.5505</v>
+        <v>15.599</v>
       </c>
       <c r="W145" s="2">
-        <v>-88.004800000000003</v>
-      </c>
+        <v>-88.659800000000004</v>
+      </c>
+      <c r="AA145" s="8"/>
     </row>
     <row r="146" spans="1:27">
       <c r="A146" s="1">
-        <v>34671</v>
+        <v>34726</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>23</v>
@@ -11542,43 +11600,43 @@
         <v>3</v>
       </c>
       <c r="E146" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I146" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M146" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="P146" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q146" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>35</v>
@@ -11587,18 +11645,18 @@
         <v>36</v>
       </c>
       <c r="U146" s="1" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="V146" s="2">
-        <v>15.5989</v>
+        <v>15.6119</v>
       </c>
       <c r="W146" s="2">
-        <v>-87.208799999999997</v>
-      </c>
-    </row>
-    <row r="147" spans="1:27" ht="15">
+        <v>-87.956299999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27">
       <c r="A147" s="1">
-        <v>34675</v>
+        <v>35080</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>23</v>
@@ -11622,31 +11680,31 @@
         <v>27</v>
       </c>
       <c r="I147" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="L147" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M147" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="O147" s="1" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="P147" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q147" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="R147" s="1" t="s">
         <v>35</v>
@@ -11655,19 +11713,18 @@
         <v>36</v>
       </c>
       <c r="U147" s="1" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="V147" s="2">
-        <v>15.599</v>
+        <v>15.7738</v>
       </c>
       <c r="W147" s="2">
-        <v>-88.659800000000004</v>
-      </c>
-      <c r="AA147" s="8"/>
+        <v>-87.475499999999997</v>
+      </c>
     </row>
     <row r="148" spans="1:27">
       <c r="A148" s="1">
-        <v>34726</v>
+        <v>35085</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>23</v>
@@ -11679,25 +11736,25 @@
         <v>3</v>
       </c>
       <c r="E148" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I148" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>30</v>
@@ -11706,16 +11763,16 @@
         <v>1</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="P148" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q148" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="R148" s="1" t="s">
         <v>35</v>
@@ -11724,18 +11781,18 @@
         <v>36</v>
       </c>
       <c r="U148" s="1" t="s">
-        <v>56</v>
+        <v>183</v>
       </c>
       <c r="V148" s="2">
-        <v>15.6119</v>
+        <v>15.7744</v>
       </c>
       <c r="W148" s="2">
-        <v>-87.956299999999999</v>
+        <v>-87.446799999999996</v>
       </c>
     </row>
     <row r="149" spans="1:27">
       <c r="A149" s="1">
-        <v>35080</v>
+        <v>35108</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>23</v>
@@ -11759,13 +11816,13 @@
         <v>27</v>
       </c>
       <c r="I149" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L149" s="1" t="s">
         <v>30</v>
@@ -11774,16 +11831,16 @@
         <v>1</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P149" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q149" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R149" s="1" t="s">
         <v>35</v>
@@ -11792,18 +11849,18 @@
         <v>36</v>
       </c>
       <c r="U149" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="V149" s="2">
-        <v>15.7738</v>
+        <v>15.5989</v>
       </c>
       <c r="W149" s="2">
-        <v>-87.475499999999997</v>
+        <v>-87.208799999999997</v>
       </c>
     </row>
     <row r="150" spans="1:27">
       <c r="A150" s="1">
-        <v>35085</v>
+        <v>35182</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>23</v>
@@ -11860,18 +11917,18 @@
         <v>36</v>
       </c>
       <c r="U150" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="V150" s="2">
-        <v>15.7744</v>
+        <v>15.781700000000001</v>
       </c>
       <c r="W150" s="2">
-        <v>-87.446799999999996</v>
+        <v>-87.453400000000002</v>
       </c>
     </row>
     <row r="151" spans="1:27">
       <c r="A151" s="1">
-        <v>35108</v>
+        <v>35243</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>23</v>
@@ -11895,13 +11952,13 @@
         <v>27</v>
       </c>
       <c r="I151" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L151" s="1" t="s">
         <v>30</v>
@@ -11910,16 +11967,16 @@
         <v>1</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P151" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q151" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="R151" s="1" t="s">
         <v>35</v>
@@ -11928,18 +11985,18 @@
         <v>36</v>
       </c>
       <c r="U151" s="1" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="V151" s="2">
-        <v>15.5989</v>
+        <v>15.783300000000001</v>
       </c>
       <c r="W151" s="2">
-        <v>-87.208799999999997</v>
+        <v>-87.452100000000002</v>
       </c>
     </row>
     <row r="152" spans="1:27">
       <c r="A152" s="1">
-        <v>35182</v>
+        <v>35246</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>23</v>
@@ -11996,18 +12053,18 @@
         <v>36</v>
       </c>
       <c r="U152" s="1" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="V152" s="2">
-        <v>15.781700000000001</v>
+        <v>15.7834</v>
       </c>
       <c r="W152" s="2">
-        <v>-87.453400000000002</v>
+        <v>-87.449399999999997</v>
       </c>
     </row>
     <row r="153" spans="1:27">
       <c r="A153" s="1">
-        <v>35243</v>
+        <v>35257</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>23</v>
@@ -12031,13 +12088,13 @@
         <v>27</v>
       </c>
       <c r="I153" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
@@ -12046,16 +12103,16 @@
         <v>1</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>35</v>
@@ -12064,18 +12121,18 @@
         <v>36</v>
       </c>
       <c r="U153" s="1" t="s">
-        <v>189</v>
+        <v>41</v>
       </c>
       <c r="V153" s="2">
-        <v>15.783300000000001</v>
+        <v>15.7836</v>
       </c>
       <c r="W153" s="2">
-        <v>-87.452100000000002</v>
+        <v>-86.792500000000004</v>
       </c>
     </row>
     <row r="154" spans="1:27">
       <c r="A154" s="1">
-        <v>35246</v>
+        <v>35269</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>23</v>
@@ -12132,18 +12189,18 @@
         <v>36</v>
       </c>
       <c r="U154" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="V154" s="2">
-        <v>15.7834</v>
+        <v>15.783899999999999</v>
       </c>
       <c r="W154" s="2">
-        <v>-87.449399999999997</v>
+        <v>-87.449700000000007</v>
       </c>
     </row>
     <row r="155" spans="1:27">
       <c r="A155" s="1">
-        <v>35257</v>
+        <v>35275</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>23</v>
@@ -12167,13 +12224,13 @@
         <v>27</v>
       </c>
       <c r="I155" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12182,16 +12239,16 @@
         <v>1</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>35</v>
@@ -12203,15 +12260,15 @@
         <v>41</v>
       </c>
       <c r="V155" s="2">
-        <v>15.7836</v>
+        <v>15.7841</v>
       </c>
       <c r="W155" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.450699999999998</v>
       </c>
     </row>
     <row r="156" spans="1:27">
       <c r="A156" s="1">
-        <v>35269</v>
+        <v>35290</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>23</v>
@@ -12268,18 +12325,18 @@
         <v>36</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>49</v>
+        <v>190</v>
       </c>
       <c r="V156" s="2">
-        <v>15.783899999999999</v>
+        <v>15.7845</v>
       </c>
       <c r="W156" s="2">
-        <v>-87.449700000000007</v>
+        <v>-87.451599999999999</v>
       </c>
     </row>
     <row r="157" spans="1:27">
       <c r="A157" s="1">
-        <v>35275</v>
+        <v>35304</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>23</v>
@@ -12303,13 +12360,13 @@
         <v>27</v>
       </c>
       <c r="I157" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>30</v>
@@ -12318,16 +12375,16 @@
         <v>1</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q157" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>35</v>
@@ -12336,18 +12393,18 @@
         <v>36</v>
       </c>
       <c r="U157" s="1" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
       <c r="V157" s="2">
-        <v>15.7841</v>
+        <v>15.784800000000001</v>
       </c>
       <c r="W157" s="2">
-        <v>-87.450699999999998</v>
+        <v>-86.792900000000003</v>
       </c>
     </row>
     <row r="158" spans="1:27">
       <c r="A158" s="1">
-        <v>35290</v>
+        <v>35307</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>23</v>
@@ -12371,13 +12428,13 @@
         <v>27</v>
       </c>
       <c r="I158" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>30</v>
@@ -12386,16 +12443,16 @@
         <v>1</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P158" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q158" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>35</v>
@@ -12403,19 +12460,19 @@
       <c r="S158" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U158" s="1" t="s">
-        <v>190</v>
+      <c r="U158" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="V158" s="2">
-        <v>15.7845</v>
+        <v>15.7849</v>
       </c>
       <c r="W158" s="2">
-        <v>-87.451599999999999</v>
+        <v>-86.791899999999998</v>
       </c>
     </row>
     <row r="159" spans="1:27">
       <c r="A159" s="1">
-        <v>35304</v>
+        <v>35819</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>23</v>
@@ -12427,13 +12484,13 @@
         <v>3</v>
       </c>
       <c r="E159" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12442,10 +12499,10 @@
         <v>1</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
@@ -12454,16 +12511,16 @@
         <v>1</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q159" s="1" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="R159" s="1" t="s">
         <v>35</v>
@@ -12472,18 +12529,18 @@
         <v>36</v>
       </c>
       <c r="U159" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="V159" s="2">
-        <v>15.784800000000001</v>
+        <v>16.319299999999998</v>
       </c>
       <c r="W159" s="2">
-        <v>-86.792900000000003</v>
-      </c>
-    </row>
-    <row r="160" spans="1:27">
+        <v>-86.538700000000006</v>
+      </c>
+    </row>
+    <row r="160" spans="1:27" ht="15">
       <c r="A160" s="1">
-        <v>35307</v>
+        <v>35879</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>23</v>
@@ -12495,25 +12552,25 @@
         <v>3</v>
       </c>
       <c r="E160" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I160" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>30</v>
@@ -12522,16 +12579,16 @@
         <v>1</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="P160" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q160" s="1" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="R160" s="1" t="s">
         <v>35</v>
@@ -12543,15 +12600,16 @@
         <v>78</v>
       </c>
       <c r="V160" s="2">
-        <v>15.7849</v>
+        <v>16.442499999999999</v>
       </c>
       <c r="W160" s="2">
-        <v>-86.791899999999998</v>
-      </c>
-    </row>
-    <row r="161" spans="1:27">
+        <v>-85.887699999999995</v>
+      </c>
+      <c r="AA160" s="8"/>
+    </row>
+    <row r="161" spans="1:23">
       <c r="A161" s="1">
-        <v>35819</v>
+        <v>50001</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>23</v>
@@ -12563,25 +12621,25 @@
         <v>3</v>
       </c>
       <c r="E161" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>192</v>
+        <v>79</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I161" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
@@ -12590,16 +12648,16 @@
         <v>1</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="P161" s="1" t="s">
-        <v>33</v>
+        <v>203</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>197</v>
+        <v>111</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>35</v>
@@ -12608,18 +12666,18 @@
         <v>36</v>
       </c>
       <c r="U161" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="V161" s="2">
-        <v>16.319299999999998</v>
+        <v>14.5968988</v>
       </c>
       <c r="W161" s="2">
-        <v>-86.538700000000006</v>
-      </c>
-    </row>
-    <row r="162" spans="1:27" ht="15">
+        <v>-87.831554999999994</v>
+      </c>
+    </row>
+    <row r="162" spans="1:23">
       <c r="A162" s="1">
-        <v>35879</v>
+        <v>50002</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>23</v>
@@ -12631,25 +12689,25 @@
         <v>3</v>
       </c>
       <c r="E162" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>192</v>
+        <v>79</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I162" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>200</v>
+        <v>109</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
@@ -12658,16 +12716,16 @@
         <v>1</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>201</v>
+        <v>110</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>200</v>
+        <v>109</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>202</v>
+        <v>111</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>35</v>
@@ -12675,21 +12733,1181 @@
       <c r="S162" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U162" s="7" t="s">
-        <v>78</v>
+      <c r="U162" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="V162" s="2">
-        <v>16.442499999999999</v>
+        <v>14.597671699999999</v>
       </c>
       <c r="W162" s="2">
-        <v>-85.887699999999995</v>
-      </c>
-      <c r="AA162" s="8"/>
-    </row>
+        <v>-87.831420600000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:23" ht="15">
+      <c r="A163" s="1">
+        <v>50003</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" s="1">
+        <v>3</v>
+      </c>
+      <c r="E163" s="1">
+        <v>3</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I163" s="1">
+        <v>18</v>
+      </c>
+      <c r="J163" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M163" s="1">
+        <v>1</v>
+      </c>
+      <c r="N163" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P163" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q163" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S163" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U163" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="V163" s="2">
+        <v>14.596547299999999</v>
+      </c>
+      <c r="W163" s="2">
+        <v>-87.828834999999998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:23">
+      <c r="A164" s="1">
+        <v>50004</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D164" s="1">
+        <v>3</v>
+      </c>
+      <c r="E164" s="1">
+        <v>3</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I164" s="1">
+        <v>18</v>
+      </c>
+      <c r="J164" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M164" s="1">
+        <v>1</v>
+      </c>
+      <c r="N164" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P164" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q164" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S164" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U164" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V164" s="2">
+        <v>14.596470500000001</v>
+      </c>
+      <c r="W164" s="2">
+        <v>-87.8321428</v>
+      </c>
+    </row>
+    <row r="165" spans="1:23">
+      <c r="A165" s="1">
+        <v>50005</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D165" s="1">
+        <v>3</v>
+      </c>
+      <c r="E165" s="1">
+        <v>3</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I165" s="1">
+        <v>18</v>
+      </c>
+      <c r="J165" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K165" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M165" s="1">
+        <v>1</v>
+      </c>
+      <c r="N165" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q165" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S165" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U165" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V165" s="2">
+        <v>14.6011212</v>
+      </c>
+      <c r="W165" s="2">
+        <v>-87.842944000000003</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23" ht="15">
+      <c r="A166" s="1">
+        <v>50006</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166" s="1">
+        <v>3</v>
+      </c>
+      <c r="E166" s="1">
+        <v>3</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I166" s="1">
+        <v>18</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L166" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M166" s="1">
+        <v>1</v>
+      </c>
+      <c r="N166" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O166" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P166" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q166" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S166" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U166" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="V166" s="2">
+        <v>14.596408200000001</v>
+      </c>
+      <c r="W166" s="2">
+        <v>-87.8313287</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23">
+      <c r="A167" s="1">
+        <v>50007</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167" s="1">
+        <v>3</v>
+      </c>
+      <c r="E167" s="1">
+        <v>3</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I167" s="1">
+        <v>18</v>
+      </c>
+      <c r="J167" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L167" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M167" s="1">
+        <v>1</v>
+      </c>
+      <c r="N167" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P167" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q167" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S167" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U167" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="V167" s="2">
+        <v>14.5942943</v>
+      </c>
+      <c r="W167" s="2">
+        <v>-87.829985600000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:23">
+      <c r="A168" s="1">
+        <v>50008</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D168" s="1">
+        <v>3</v>
+      </c>
+      <c r="E168" s="1">
+        <v>3</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I168" s="1">
+        <v>18</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M168" s="1">
+        <v>1</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O168" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P168" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q168" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S168" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U168" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="V168" s="2">
+        <v>14.5972314</v>
+      </c>
+      <c r="W168" s="2">
+        <v>-87.838980399999997</v>
+      </c>
+    </row>
+    <row r="169" spans="1:23">
+      <c r="A169" s="1">
+        <v>50009</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D169" s="1">
+        <v>3</v>
+      </c>
+      <c r="E169" s="1">
+        <v>3</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I169" s="1">
+        <v>18</v>
+      </c>
+      <c r="J169" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L169" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M169" s="1">
+        <v>1</v>
+      </c>
+      <c r="N169" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O169" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P169" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q169" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R169" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S169" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U169" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="V169" s="2">
+        <v>14.601276</v>
+      </c>
+      <c r="W169" s="2">
+        <v>-87.837087800000006</v>
+      </c>
+    </row>
+    <row r="170" spans="1:23">
+      <c r="A170" s="1">
+        <v>50010</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170" s="1">
+        <v>3</v>
+      </c>
+      <c r="E170" s="1">
+        <v>3</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I170" s="1">
+        <v>18</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M170" s="1">
+        <v>1</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O170" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q170" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R170" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S170" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U170" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V170" s="2">
+        <v>14.593768300000001</v>
+      </c>
+      <c r="W170" s="2">
+        <v>-87.831689600000004</v>
+      </c>
+    </row>
+    <row r="171" spans="1:23">
+      <c r="A171" s="1">
+        <v>50011</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" s="1">
+        <v>3</v>
+      </c>
+      <c r="E171" s="1">
+        <v>3</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I171" s="1">
+        <v>18</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M171" s="1">
+        <v>1</v>
+      </c>
+      <c r="N171" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q171" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R171" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S171" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U171" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="V171" s="2">
+        <v>14.587884600000001</v>
+      </c>
+      <c r="W171" s="2">
+        <v>-87.836289500000007</v>
+      </c>
+    </row>
+    <row r="172" spans="1:23">
+      <c r="A172" s="1">
+        <v>50012</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D172" s="1">
+        <v>3</v>
+      </c>
+      <c r="E172" s="1">
+        <v>3</v>
+      </c>
+      <c r="F172" s="1">
+        <v>3</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I172" s="1">
+        <v>18</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M172" s="1">
+        <v>1</v>
+      </c>
+      <c r="N172" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q172" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S172" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U172" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V172" s="2">
+        <v>14.5971791</v>
+      </c>
+      <c r="W172" s="2">
+        <v>-87.838133499999998</v>
+      </c>
+    </row>
+    <row r="173" spans="1:23">
+      <c r="A173" s="1">
+        <v>50013</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D173" s="1">
+        <v>3</v>
+      </c>
+      <c r="E173" s="1">
+        <v>3</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I173" s="1">
+        <v>18</v>
+      </c>
+      <c r="J173" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L173" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M173" s="1">
+        <v>1</v>
+      </c>
+      <c r="N173" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O173" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P173" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q173" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R173" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S173" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U173" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="V173" s="2">
+        <v>14.5936644</v>
+      </c>
+      <c r="W173" s="2">
+        <v>-87.831741600000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23">
+      <c r="A174" s="1">
+        <v>50014</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D174" s="1">
+        <v>3</v>
+      </c>
+      <c r="E174" s="1">
+        <v>3</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I174" s="1">
+        <v>18</v>
+      </c>
+      <c r="J174" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K174" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M174" s="1">
+        <v>1</v>
+      </c>
+      <c r="N174" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O174" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P174" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q174" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R174" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S174" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U174" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="V174" s="2">
+        <v>14.598122099999999</v>
+      </c>
+      <c r="W174" s="2">
+        <v>-87.831477599999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23">
+      <c r="A175" s="1">
+        <v>50015</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D175" s="1">
+        <v>3</v>
+      </c>
+      <c r="E175" s="1">
+        <v>3</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I175" s="1">
+        <v>18</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K175" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L175" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M175" s="1">
+        <v>1</v>
+      </c>
+      <c r="N175" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O175" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P175" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q175" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R175" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S175" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U175" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="V175" s="2">
+        <v>14.596882600000001</v>
+      </c>
+      <c r="W175" s="2">
+        <v>-87.840906599999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:23">
+      <c r="A176" s="1">
+        <v>50016</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D176" s="1">
+        <v>3</v>
+      </c>
+      <c r="E176" s="1">
+        <v>3</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I176" s="1">
+        <v>18</v>
+      </c>
+      <c r="J176" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K176" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L176" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M176" s="1">
+        <v>1</v>
+      </c>
+      <c r="N176" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O176" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P176" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q176" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R176" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S176" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U176" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="V176" s="2">
+        <v>14.5838927</v>
+      </c>
+      <c r="W176" s="2">
+        <v>-87.846112700000006</v>
+      </c>
+    </row>
+    <row r="177" spans="1:23">
+      <c r="A177" s="1">
+        <v>50017</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D177" s="1">
+        <v>3</v>
+      </c>
+      <c r="E177" s="1">
+        <v>3</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I177" s="1">
+        <v>18</v>
+      </c>
+      <c r="J177" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K177" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L177" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M177" s="1">
+        <v>1</v>
+      </c>
+      <c r="N177" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O177" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P177" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q177" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R177" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S177" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U177" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V177" s="2">
+        <v>14.5993443</v>
+      </c>
+      <c r="W177" s="2">
+        <v>-87.8429754</v>
+      </c>
+    </row>
+    <row r="178" spans="1:23">
+      <c r="A178" s="1">
+        <v>50018</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D178" s="1">
+        <v>3</v>
+      </c>
+      <c r="E178" s="1">
+        <v>3</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I178" s="1">
+        <v>18</v>
+      </c>
+      <c r="J178" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K178" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L178" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M178" s="1">
+        <v>1</v>
+      </c>
+      <c r="N178" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O178" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P178" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q178" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R178" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S178" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U178" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="V178" s="2">
+        <v>14.5966769</v>
+      </c>
+      <c r="W178" s="2">
+        <v>-87.832520599999995</v>
+      </c>
+    </row>
+    <row r="179" spans="1:23">
+      <c r="A179" s="1">
+        <v>50019</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D179" s="1">
+        <v>3</v>
+      </c>
+      <c r="E179" s="1">
+        <v>3</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I179" s="1">
+        <v>18</v>
+      </c>
+      <c r="J179" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K179" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M179" s="1">
+        <v>1</v>
+      </c>
+      <c r="N179" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O179" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P179" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q179" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R179" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S179" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U179" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="V179" s="2">
+        <v>14.5967611</v>
+      </c>
+      <c r="W179" s="2">
+        <v>-87.840956000000006</v>
+      </c>
+    </row>
+    <row r="183" spans="1:23" ht="15">
+      <c r="T183" s="9"/>
+    </row>
+    <row r="184" spans="1:23" ht="15"/>
+    <row r="185" spans="1:23" ht="15"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U162">
-    <sortCondition ref="R2:R162"/>
-    <sortCondition ref="S2:S162"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U160">
+    <sortCondition ref="R2:R160"/>
+    <sortCondition ref="S2:S160"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-23-2020 04-32-04
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="639" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{133B870B-09C0-4216-8C99-C73D3287A0DA}"/>
+  <xr:revisionPtr revIDLastSave="747" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{10B773EB-B235-4AB2-8838-26CAE9EE7CA5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="FARMACIAS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$179</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$190</definedName>
     <definedName name="_xlnm.Database">FARMACIAS!$A$1:$U$160</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="246">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -697,6 +697,81 @@
   </si>
   <si>
     <t>FarmaCity Calle 21 de agosto</t>
+  </si>
+  <si>
+    <t>Gracias a Dios</t>
+  </si>
+  <si>
+    <t>Puerto Lempira</t>
+  </si>
+  <si>
+    <t>HND-0901</t>
+  </si>
+  <si>
+    <t>Clinica medica JOZAM</t>
+  </si>
+  <si>
+    <t>Olancho</t>
+  </si>
+  <si>
+    <t>Catacamas</t>
+  </si>
+  <si>
+    <t>HND-1503</t>
+  </si>
+  <si>
+    <t>Farmacia y Clínica Eva</t>
+  </si>
+  <si>
+    <t>La union</t>
+  </si>
+  <si>
+    <t>La Union</t>
+  </si>
+  <si>
+    <t>HND-1513</t>
+  </si>
+  <si>
+    <t>Farmacia Regis La Unión</t>
+  </si>
+  <si>
+    <t>Dulce Nombre de Culmi</t>
+  </si>
+  <si>
+    <t>HND-1505</t>
+  </si>
+  <si>
+    <t>Farmacia Regis Culmi</t>
+  </si>
+  <si>
+    <t>Gualaco</t>
+  </si>
+  <si>
+    <t>HND-1508</t>
+  </si>
+  <si>
+    <t>Farmatodo</t>
+  </si>
+  <si>
+    <t>Farmacia Sol Farma</t>
+  </si>
+  <si>
+    <t>Farmacia Regis Gualaco</t>
+  </si>
+  <si>
+    <t>Juticalpa</t>
+  </si>
+  <si>
+    <t>HND-1501</t>
+  </si>
+  <si>
+    <t>Farmacia Santa Gertrudis</t>
+  </si>
+  <si>
+    <t>Farmacias del ahorro #88</t>
+  </si>
+  <si>
+    <t>Farmacia Y Clinica Samaritana</t>
   </si>
 </sst>
 </file>
@@ -1357,8 +1432,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W179" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W179" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W190" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W190" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W160">
     <sortCondition ref="A1:A160"/>
   </sortState>
@@ -1688,11 +1763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA185"/>
+  <dimension ref="A1:AA190"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
+      <pane ySplit="1" topLeftCell="P177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V190" sqref="V190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -13371,8 +13446,8 @@
       <c r="E172" s="1">
         <v>3</v>
       </c>
-      <c r="F172" s="1">
-        <v>3</v>
+      <c r="F172" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>80</v>
@@ -13899,11 +13974,754 @@
         <v>-87.840956000000006</v>
       </c>
     </row>
+    <row r="180" spans="1:23">
+      <c r="A180" s="1">
+        <v>50020</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D180" s="1">
+        <v>3</v>
+      </c>
+      <c r="E180" s="1">
+        <v>9</v>
+      </c>
+      <c r="F180" s="1">
+        <v>9</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I180" s="1">
+        <v>1</v>
+      </c>
+      <c r="J180" s="1">
+        <v>901</v>
+      </c>
+      <c r="K180" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L180" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M180" s="1">
+        <v>1</v>
+      </c>
+      <c r="N180" s="1">
+        <v>90101</v>
+      </c>
+      <c r="O180" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P180" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q180" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R180" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S180" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U180" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V180" s="2">
+        <v>15.257429999999999</v>
+      </c>
+      <c r="W180" s="2">
+        <v>-83.780617000000007</v>
+      </c>
+    </row>
+    <row r="181" spans="1:23">
+      <c r="A181" s="1">
+        <v>50021</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D181" s="1">
+        <v>3</v>
+      </c>
+      <c r="E181" s="1">
+        <v>9</v>
+      </c>
+      <c r="F181" s="1">
+        <v>9</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I181" s="1">
+        <v>1</v>
+      </c>
+      <c r="J181" s="1">
+        <v>901</v>
+      </c>
+      <c r="K181" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L181" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M181" s="1">
+        <v>1</v>
+      </c>
+      <c r="N181" s="1">
+        <v>90101</v>
+      </c>
+      <c r="O181" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P181" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q181" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R181" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S181" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U181" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V181" s="2">
+        <v>15.266281599999999</v>
+      </c>
+      <c r="W181" s="2">
+        <v>-83.772572199999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:23">
+      <c r="A182" s="1">
+        <v>50022</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D182" s="1">
+        <v>3</v>
+      </c>
+      <c r="E182" s="1">
+        <v>15</v>
+      </c>
+      <c r="F182" s="1">
+        <v>15</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I182" s="1">
+        <v>3</v>
+      </c>
+      <c r="J182" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K182" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L182" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M182" s="1">
+        <v>1</v>
+      </c>
+      <c r="N182" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O182" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P182" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q182" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R182" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S182" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U182" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V182" s="2">
+        <v>14.8959817</v>
+      </c>
+      <c r="W182" s="2">
+        <v>-85.7856022</v>
+      </c>
+    </row>
     <row r="183" spans="1:23" ht="15">
-      <c r="T183" s="9"/>
-    </row>
-    <row r="184" spans="1:23" ht="15"/>
-    <row r="185" spans="1:23" ht="15"/>
+      <c r="A183" s="1">
+        <v>50023</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D183" s="1">
+        <v>3</v>
+      </c>
+      <c r="E183" s="1">
+        <v>15</v>
+      </c>
+      <c r="F183" s="1">
+        <v>15</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I183" s="1">
+        <v>13</v>
+      </c>
+      <c r="J183" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K183" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L183" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M183" s="1">
+        <v>1</v>
+      </c>
+      <c r="N183" s="1">
+        <v>151301</v>
+      </c>
+      <c r="O183" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P183" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q183" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R183" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S183" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U183" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="V183" s="2">
+        <v>15.022712</v>
+      </c>
+      <c r="W183" s="2">
+        <v>-86.709926899999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:23" ht="15">
+      <c r="A184" s="1">
+        <v>50024</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D184" s="1">
+        <v>3</v>
+      </c>
+      <c r="E184" s="1">
+        <v>15</v>
+      </c>
+      <c r="F184" s="1">
+        <v>15</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I184" s="1">
+        <v>5</v>
+      </c>
+      <c r="J184" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K184" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="L184" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M184" s="1">
+        <v>1</v>
+      </c>
+      <c r="N184" s="1">
+        <v>150501</v>
+      </c>
+      <c r="O184" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="P184" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q184" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="R184" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S184" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U184" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="V184" s="2">
+        <v>15.0837658</v>
+      </c>
+      <c r="W184" s="2">
+        <v>-85.556933099999995</v>
+      </c>
+    </row>
+    <row r="185" spans="1:23" ht="15">
+      <c r="A185" s="1">
+        <v>50025</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D185" s="1">
+        <v>3</v>
+      </c>
+      <c r="E185" s="1">
+        <v>15</v>
+      </c>
+      <c r="F185" s="1">
+        <v>15</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I185" s="1">
+        <v>8</v>
+      </c>
+      <c r="J185" s="1">
+        <v>1508</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L185" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M185" s="1">
+        <v>1</v>
+      </c>
+      <c r="N185" s="1">
+        <v>150801</v>
+      </c>
+      <c r="O185" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P185" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q185" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="R185" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S185" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U185" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="V185" s="2">
+        <v>15.025620699999999</v>
+      </c>
+      <c r="W185" s="2">
+        <v>-86.071155000000005</v>
+      </c>
+    </row>
+    <row r="186" spans="1:23">
+      <c r="A186" s="1">
+        <v>50026</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D186" s="1">
+        <v>3</v>
+      </c>
+      <c r="E186" s="1">
+        <v>15</v>
+      </c>
+      <c r="F186" s="1">
+        <v>15</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I186" s="1">
+        <v>8</v>
+      </c>
+      <c r="J186" s="1">
+        <v>1508</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L186" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M186" s="1">
+        <v>1</v>
+      </c>
+      <c r="N186" s="1">
+        <v>150801</v>
+      </c>
+      <c r="O186" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P186" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q186" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="R186" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S186" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U186" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="V186" s="2">
+        <v>15.023555399999999</v>
+      </c>
+      <c r="W186" s="2">
+        <v>-86.069538199999997</v>
+      </c>
+    </row>
+    <row r="187" spans="1:23">
+      <c r="A187" s="1">
+        <v>50027</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D187" s="1">
+        <v>3</v>
+      </c>
+      <c r="E187" s="1">
+        <v>15</v>
+      </c>
+      <c r="F187" s="1">
+        <v>15</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I187" s="1">
+        <v>8</v>
+      </c>
+      <c r="J187" s="1">
+        <v>1508</v>
+      </c>
+      <c r="K187" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L187" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M187" s="1">
+        <v>1</v>
+      </c>
+      <c r="N187" s="1">
+        <v>150801</v>
+      </c>
+      <c r="O187" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P187" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q187" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="R187" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S187" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U187" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V187" s="2">
+        <v>15.027041000000001</v>
+      </c>
+      <c r="W187" s="2">
+        <v>-86.070589999999996</v>
+      </c>
+    </row>
+    <row r="188" spans="1:23">
+      <c r="A188" s="1">
+        <v>50028</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D188" s="1">
+        <v>3</v>
+      </c>
+      <c r="E188" s="1">
+        <v>15</v>
+      </c>
+      <c r="F188" s="1">
+        <v>15</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I188" s="1">
+        <v>1</v>
+      </c>
+      <c r="J188" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L188" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M188" s="1">
+        <v>1</v>
+      </c>
+      <c r="N188" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O188" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P188" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q188" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R188" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S188" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U188" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="V188" s="2">
+        <v>14.670859399999999</v>
+      </c>
+      <c r="W188" s="2">
+        <v>-86.220775200000006</v>
+      </c>
+    </row>
+    <row r="189" spans="1:23">
+      <c r="A189" s="1">
+        <v>50029</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D189" s="1">
+        <v>3</v>
+      </c>
+      <c r="E189" s="1">
+        <v>15</v>
+      </c>
+      <c r="F189" s="1">
+        <v>15</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I189" s="1">
+        <v>3</v>
+      </c>
+      <c r="J189" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K189" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L189" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M189" s="1">
+        <v>1</v>
+      </c>
+      <c r="N189" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O189" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P189" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q189" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R189" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S189" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U189" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="V189" s="2">
+        <v>14.8461187</v>
+      </c>
+      <c r="W189" s="2">
+        <v>-85.890722999999994</v>
+      </c>
+    </row>
+    <row r="190" spans="1:23">
+      <c r="A190" s="1">
+        <v>50030</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D190" s="1">
+        <v>3</v>
+      </c>
+      <c r="E190" s="1">
+        <v>15</v>
+      </c>
+      <c r="F190" s="1">
+        <v>15</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I190" s="1">
+        <v>3</v>
+      </c>
+      <c r="J190" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L190" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M190" s="1">
+        <v>1</v>
+      </c>
+      <c r="N190" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P190" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q190" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R190" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S190" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U190" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="V190" s="2">
+        <v>14.8461187</v>
+      </c>
+      <c r="W190" s="2">
+        <v>-85.896107000000001</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U160">
     <sortCondition ref="R2:R160"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-24-2020 10-36-39
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1076" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E23114E6-42EE-4963-A0BA-734DCF680552}"/>
+  <xr:revisionPtr revIDLastSave="1079" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12CF6402-D76C-49A5-80CF-C39B3C89AB4E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1889,8 +1889,8 @@
   <dimension ref="A1:AA235"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="Q223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S235" sqref="S235"/>
+      <pane ySplit="1" topLeftCell="T128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V144" sqref="V144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -1919,7 +1919,7 @@
     <col min="23" max="23" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="5" customFormat="1">
+    <row r="1" spans="1:27" s="5" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:27">
       <c r="A2" s="1">
         <v>17840</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>-87.057100000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <v>18049</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>-87.179100000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <v>18065</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>-87.175299999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <v>24496</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>-87.232399999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <v>24554</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>-87.211399999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <v>24613</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>-87.2226</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <v>24618</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>-87.222300000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:27">
       <c r="A9" s="1">
         <v>24623</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>-87.222099999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:27">
       <c r="A10" s="1">
         <v>24627</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>-87.229299999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:27">
       <c r="A11" s="1">
         <v>24646</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>-87.189599999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" s="1">
         <v>24650</v>
       </c>
@@ -2737,8 +2737,9 @@
       <c r="W12" s="2">
         <v>-87.189400000000006</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="AA12" s="8"/>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="1">
         <v>24656</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>-87.220600000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:27">
       <c r="A14" s="1">
         <v>24667</v>
       </c>
@@ -2871,10 +2872,10 @@
         <v>14.0601</v>
       </c>
       <c r="W14" s="2">
-        <v>-83.400400000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
+        <v>-87.400400000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="1">
         <v>24701</v>
       </c>
@@ -2942,7 +2943,7 @@
         <v>-87.209599999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:27">
       <c r="A16" s="1">
         <v>24711</v>
       </c>
@@ -11712,7 +11713,7 @@
         <v>15.5989</v>
       </c>
       <c r="W144" s="2">
-        <v>-87.208799999999997</v>
+        <v>-87.102687200000005</v>
       </c>
     </row>
     <row r="145" spans="1:27" ht="15">

</xml_diff>